<commit_message>
Ukrainian for Russian, Foundsource filters, Regional zoom, Animated phrases and so on...
1. Russian defaulted browsers see Ukrainian translation now;
2. New filter design and function. Foundsource filters added to regional chart;
3. Datazoom bar added to scale regional chart;
4. Animated phrases for required supplies if a region has enough vaccine.
</commit_message>
<xml_diff>
--- a/Results/Коди ЄДРПОУ з багатьма варіантами назв закладів.xlsx
+++ b/Results/Коди ЄДРПОУ з багатьма варіантами назв закладів.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B79"/>
+  <dimension ref="A1:B88"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -460,922 +460,1030 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>1992953</t>
+          <t>1993486</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>[['КНП  ОРІХІВСЬКА БАГАТОПРОФІЛЬНА ЛІКАРНЯ ІНТЕНСИВНОГО ЛІКУВАННЯ ОРІХІВСЬКОЇ МІСЬКОЇ РАДИ', 9], ['ДУ «ЗАПОРІЗЬКИЙ  ОЦКПХ  МОЗ »)', 1]]</t>
+          <t>[['КНП\'\'Тисменицька міська лікарня"Тисменицької міської ради', 14], ['КНП Тисменицька міська лікарня Тисменицької міської ради', 1]]</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>1993486</t>
+          <t>1995290</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>[['КНП\'\'Тисменицька міська лікарня"Тисменицької міської ради', 9], ['КНП Тисменицька міська лікарня Тисменицької міської ради', 1]]</t>
+          <t>[['КНП "Петрівська Центральна лікарня" Петрівської селищної ради', 1], ['КНП "Петрівська Центральна лікарня" Петрівської районної ради', 1]]</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>1995290</t>
+          <t>1998354</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>[['КНП "Петрівська Центральна лікарня" Петрівської селищної ради', 1], ['КНП "Петрівська Центральна лікарня" Петрівської районної ради', 1]]</t>
+          <t>[['КНП "Баштанська БПЛ"', 3], ['КНП"Баштанська БПЛ', 4]]</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>1998360</t>
+          <t>1998785</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>[['КНП "Березанська ЦРЛ"', 1], ['КНП "Березанская ЦРЛ"', 3]]</t>
+          <t>[['КНП "Кодимська лікарня" Кодимської міської ради Подільського району Одеської області', 2], ['КНП "Кодимська лікарня"\n  Кодимської міської ради\n  Подільського району\n  Одеської області', 2]]</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>1998785</t>
+          <t>2004216</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>[['КНП "Кодимська лікарня" Кодимської міської ради Подільського району Одеської області', 2], ['КНП "Кодимська лікарня"\n  Кодимської міської ради\n  Подільського району\n  Одеської області', 2]]</t>
+          <t>[['КНП "Городоцька МБЛ" Городоцької міської ради', 1], ['КНП "Городоцька МБЛ"', 1], ['КНП Городоцька МБЛ', 1]]</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>2004404</t>
+          <t>2004367</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>[['КНП "Полонська МЛ ім. Н. С. Говорун"', 1], ['Комунальне некомерційне підприємство Полонської міської ради "Полонська міська багатопрофільна лікарня ім. Наталії Савеліївни Говорун"', 1]]</t>
+          <t>[['КНА "Летичівська багатопрорфільна лікарня"', 1], ['КРП "Летичівська багатопрофільна лікарня"', 1]]</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>2004812</t>
+          <t>2004404</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>[['КНП "Шепетівська багатопрофільна лікарня" Шепетівської міської ради', 2], ['КНП "Шепетівська багатопофільна лікарня" Шепетівської міської ради', 1], ['КНП"Шепетівська багатопрофільна лікарня" Шепетівської міської ради', 1]]</t>
+          <t>[['КНП "Полонська МЛ ім. Н. С. Говорун"', 1], ['Комунальне некомерційне підприємство Полонської міської ради "Полонська міська багатопрофільна лікарня ім. Наталії Савеліївни Говорун"', 1]]</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>2006194</t>
+          <t>2004812</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>[["КНП ''Коропська ЦЛ'' КСР", 1], ['КНП «Варвинська лікарня» Варвинської селищної ради Прилуцького району Чернігівської області', 1]]</t>
+          <t>[['КНП "Шепетівська багатопрофільна лікарня" Шепетівської міської ради', 2], ['КНП "Шепетівська багатопофільна лікарня" Шепетівської міської ради', 1], ['КНП"Шепетівська багатопрофільна лікарня" Шепетівської міської ради', 1]]</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>2006225</t>
+          <t>2006194</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>[["КНП ''Городнянська МЛ'' ГМР", 12], ["КНП ''Корюківська ЦРЛ'' КМР", 5]]</t>
+          <t>[["КНП ''Коропська ЦЛ'' КСР", 1], ['КНП «Варвинська лікарня» Варвинської селищної ради Прилуцького району Чернігівської області', 1]]</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>2006604</t>
+          <t>2006225</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>[["КНП ''Сновська ЦРЛ'' СМР", 1], ["КНП ''Прилуцька міська дитяча лікарня'' ПМР", 5]]</t>
+          <t>[["КНП ''Городнянська МЛ'' ГМР", 16], ["КНП ''Корюківська ЦРЛ'' КМР", 5]]</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>2006610</t>
+          <t>2006604</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>[["КНП ''Чернігівська МЛ №4'' ЧМР", 4], ['КНП «Пологовий будинок» Чернігівської міської ради', 2]]</t>
+          <t>[["КНП ''Сновська ЦРЛ'' СМР", 1], ["КНП ''Прилуцька міська дитяча лікарня'' ПМР", 5]]</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>2007259</t>
+          <t>2006610</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>[['КНП  «КМДЛ №4» КМР» м.Кривий Ріг', 2], ['КП «АМЛ «АМР» м.Апостолове', 1]]</t>
+          <t>[["КНП ''Чернігівська МЛ №4'' ЧМР", 6], ['КНП «Пологовий будинок» Чернігівської міської ради', 2]]</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>2148517983</t>
+          <t>2007259</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>[['ФОП Олійник Д.Д.', 7], ['ФОП ОЛійник Д.Д.', 1]]</t>
+          <t>[['КНП  «КМДЛ №4» КМР» м.Кривий Ріг', 2], ['КП «АМЛ «АМР» м.Апостолове', 1]]</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>22348948</t>
+          <t>2148517983</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>[['БФ ім. Митрополита А. Шептицького', 6], ['Благодійний Фонд "Шпиталь імені Митрополита Андрея Шептицького Курії Львівської Архиєпархії Української Греко-Католицької Церкви"', 8]]</t>
+          <t>[['ФОП Олійник Д.Д.', 7], ['ФОП ОЛійник Д.Д.', 1], ['ФОП олійник Д.Д.', 1]]</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>2314026147</t>
+          <t>22348948</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>[['ФОП Селезньова С. Л', 3], ['ФОП Селезньова С,Л', 1], ['ФОП Селезньова С.Л', 7]]</t>
+          <t>[['БФ ім. Митрополита А. Шептицького', 6], ['Благодійний Фонд "Шпиталь імені Митрополита Андрея Шептицького Курії Львівської Архиєпархії Української Греко-Католицької Церкви"', 8]]</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>2339913111</t>
+          <t>2314026147</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>[['ФОП "Сем\'янчук В.Б."', 8], ['ФОП Білик Роман Павлович', 9]]</t>
+          <t>[['ФОП Селезньова С. Л', 4], ['ФОП Селезньова С,Л', 1], ['ФОП Селезньова С.Л', 6]]</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>26381838</t>
+          <t>2339913111</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>[['КНП " Дитячий МЦ" КПМР', 11], ['КНП " Дитячий МЦ " КПМР', 2]]</t>
+          <t>[['ФОП "Сем\'янчук В.Б."', 9], ['ФОП Білик Роман Павлович', 10]]</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>2727016128</t>
+          <t>26381838</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>[['ФОП Ковенько Т.', 7], ['ФОП КовенькоТ.', 4]]</t>
+          <t>[['КНП " Дитячий МЦ" КПМР', 11], ['КНП " Дитячий МЦ " КПМР', 2]]</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>2798817680</t>
+          <t>2727016128</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>[['ФОП Слободянюк Л.А.', 43], ['фОП Слободянюк Л.А.', 1], ['ФОП Слободянюк Л.А. педіатр', 71]]</t>
+          <t>[['ФОП Ковенько Т.', 8], ['ФОП КовенькоТ.', 3]]</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>3146414401</t>
+          <t>2774384</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>[['ФОП Робейко Фаїна Олександрівна', 7], ['ФОП Робейко Фауна Олександрівна', 1]]</t>
+          <t>[['КП " Хмельницька міська лікарня"', 1], ['КП "Хмльницька міська лікарня"', 1], ['комунальне підприємство "Хмельницька міська лікарня"  Хмельницької міської ради', 1], ['комунальне підприємство "Хмельницька міська лікарня " Хмельницької міської ради', 1]]</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>3153200965</t>
+          <t>2798817680</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>[['ФОП ГУЗАК ОІ', 7], ['ФОп ГУЗАК ОІ', 1]]</t>
+          <t>[['ФОП Слободянюк Л.А.', 43], ['фОП Слободянюк Л.А.', 1], ['ФОП Слободянюк Л.А. педіатр', 86]]</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>3259514282</t>
+          <t>2939705320</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>[['ФОП Віннічук Юлія Валеріївна', 3], ['ФОП Віннічук Ю.В.', 15], ['ФОП ВІннічук Ю.В.', 1]]</t>
+          <t>[['ПП "Віва Клінік"', 4], ['ПП "Віва Клінік" м.Славута', 2], ['ПП " Віва Клінік"', 5]]</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>3280718060</t>
+          <t>3146414401</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>[['ФОП Гончар Інна Михайлівна', 6], ['Фоп ГоНЧАР ІМ', 1], ['Фоп ГОНЧАР ІМ', 1], ['ФОП ГОНЧАР ІМ', 4]]</t>
+          <t>[['ФОП Робейко Фаїна Олександрівна', 7], ['ФОП Робейко Фауна Олександрівна', 1]]</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>35479197</t>
+          <t>3153200965</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>[['ТОВ Клініка Свій лікар м.Дунаївці', 1], ['ТОВ"КЛІНІКА СВІЙ ЛІКАР"м.Дунаївці', 5], ['ПП"Сіліцея"', 7]]</t>
+          <t>[['ФОП ГУЗАК ОІ', 7], ['ФОп ГУЗАК ОІ', 1]]</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>37263866</t>
+          <t>3210314064</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>[['ПП"Приватна поліклініка "Малятко плюс"', 45], ['ПП "Малятко плюс"', 21]]</t>
+          <t>[['Фоп Осипенко К.В', 3], ['ФОП  Осипенко К.В', 1]]</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>37329345</t>
+          <t>3259514282</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>[['КНП"СТАРОСИНЯВСЬКИЙ ЦПМСД"', 3], ['КНП СТАРОСИНЯВСЬКИЙ ЦПМСД', 7], ['КНП "СТАРОСИНЯВСЬКИЙ ЦПМСД"', 1]]</t>
+          <t>[['ФОП Віннічук Юлія Валеріївна', 3], ['ФОП Віннічук Ю.В.', 15], ['ФОП ВІннічук Ю.В.', 1]]</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>37803420</t>
+          <t>3280718060</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>[['КНП "Мирноградський центр первинної медико-санітарної допомоги"', 1], ['КНП "Мирноградський центр первинної медико-санітарної допомоги "', 10], ['КНП " Мирноградський центр первинної медико-санітарної допомоги"', 1]]</t>
+          <t>[['ФОП Гончар Інна Михайлівна', 6], ['Фоп ГоНЧАР ІМ', 1], ['Фоп ГОНЧАР ІМ', 1], ['ФОП ГОНЧАР ІМ', 4]]</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>38073028</t>
+          <t>35479197</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>[["КНП ''Городнянський ЦПМСД'' ГМР", 12], ["КНП '' Семенівський ЦПМСД'' СМР", 3]]</t>
+          <t>[['ТОВ Клініка Свій лікар м.Дунаївці', 1], ['ТОВ"КЛІНІКА СВІЙ ЛІКАР"м.Дунаївці', 6], ['ПП"Сіліцея"', 7]]</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>38094142</t>
+          <t>37263866</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>[['КНП "Арбузинський ЦПМСД АСР"', 6], ['Арбузинський ЦПМСД', 1]]</t>
+          <t>[['ПП"Приватна поліклініка "Малятко плюс"', 45], ['ПП "Малятко плюс"', 25], ['ПП"Малятко плюс"', 2]]</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>38195551</t>
+          <t>37329345</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>[['КНП "КНП Чемеровецький центр ПМСД"', 1], ['КНП "Чемеровецький центр ПМСД"', 5], ['ТОВ "АЛМ-Поділля"', 1], ['КНП Чемеровецький центр ПМСД', 4]]</t>
+          <t>[['КНП"СТАРОСИНЯВСЬКИЙ ЦПМСД"', 3], ['КНП СТАРОСИНЯВСЬКИЙ ЦПМСД', 7], ['КНП "СТАРОСИНЯВСЬКИЙ ЦПМСД"', 1]]</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>38270455</t>
+          <t>37803420</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>[['КНП "Летичівський ЦПМСД"', 7], ['КНП"Летичівський ЦПМСД" Летичівської селищної ради', 2]]</t>
+          <t>[['КНП "Мирноградський центр первинної медико-санітарної допомоги"', 1], ['КНП "Мирноградський центр первинної медико-санітарної допомоги "', 11], ['КНП " Мирноградський центр первинної медико-санітарної допомоги"', 1]]</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>38281797</t>
+          <t>38073028</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>[['КНП"Новоронцовський районний ЦПМСД"', 8], ['КНП"Новоронцовський районний ЦПМСД"(СКЛАД)', 4]]</t>
+          <t>[["КНП ''Городнянський ЦПМСД'' ГМР", 12], ["КНП '' Семенівський ЦПМСД'' СМР", 3]]</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>38283239</t>
+          <t>38195551</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>[['КНП "Ярмолинецький центр ПМСД"', 6], ['КНП "Ярмолинецький центр ПМСД" ЯСР ХО', 1]]</t>
+          <t>[['КНП "КНП Чемеровецький центр ПМСД"', 1], ['КНП "Чемеровецький центр ПМСД"', 4], ['ТОВ "АЛМ-Поділля"', 3], ['КНП Чемеровецький центр ПМСД', 4]]</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>38297440</t>
+          <t>38270455</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>[['КНП "Білогірський ЦПМСД"', 6], ['КНП "БІЛОГІРСЬКИЙ ЦПМСД"', 3]]</t>
+          <t>[['КНП "Летичівський ЦПМСД"', 6], ['КНП"Летичівський ЦПМСД" Летичівської селищної ради', 2]]</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>38341981</t>
+          <t>38281797</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>[['КНП "Бузький РЦ ПСМД"', 8], ['КНП "Бузький РЦ ПМСД"', 1], ['КНП " Бузький ПМСД"', 1]]</t>
+          <t>[['КНП"Новоронцовський районний ЦПМСД"', 7], ['КНП"Новоронцовський районний ЦПМСД"(СКЛАД)', 4]]</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>38402043</t>
+          <t>38283239</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>[['КП КНП Шепетівський Центр ПМСД', 1], ['КП "КПН Шепетівський Центр ПМСД"', 2], ['КП"КНП Шепетівський ЦентрПМСД', 1], ['КП"КНП Шепетівський Центр ПМСД"', 6], ['КП "КНП Шепетівський Центр ПМСД"', 9], ['КП "КНП Шепетівський Центр ПМСД', 3]]</t>
+          <t>[['КНП "Ярмолинецький центр ПМСД"', 5], ['КНП "Ярмолинецький центр ПМСД" ЯСР ХО', 1]]</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>38453281</t>
+          <t>38297440</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>[["КНП ''Борзнянський ЦПМСД'' БМР", 3], ["КНП ''Прилуцький міський ЦПМСД''", 2]]</t>
+          <t>[['КНП "Білогірський ЦПМСД"', 6], ['КНП "БІЛОГІРСЬКИЙ ЦПМСД"', 3]]</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>38458316</t>
+          <t>38313933</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>[['ДУ "Миколаївський ОЦКПХ"', 4], ['ДУ"Миколаївський ОЦКПХ', 5]]</t>
+          <t>[['КП"Первомайський РЦПМСД', 10], ['КОМУНАЛЬНЕ ПІДПРИЄМСТВО «КАМ’ЯНОПО\xadТОКІВСЬКИЙ ЦЕНТР ПЕРВИННОЇ МЕДИКО-САНІТАРНОЇ ДОПОМОГИ»', 10]]</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>38462249</t>
+          <t>38341981</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>[['КНП «Макарівський ЦПМСД» Макарівської селищної ради', 8], ['КНП "Макарівський ЦПМСД" Макарівської селищної ради', 3]]</t>
+          <t>[['КНП "Бузький РЦ ПСМД"', 8], ['КНП "Бузький РЦ ПМСД"', 1], ['КНП " Бузький ПМСД"', 6]]</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>38469307</t>
+          <t>38363607</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>[['КНП "Центр ПМД Хмельницького району"', 14], ['КНП "ЦПМД Хмельницького району"', 1], ['КНП"ЦПМД Хмельницького району"', 1]]</t>
+          <t>[['КНП"Братський ЦПМСД"', 10], ['кнп "Братський ЦПМСД"', 1]]</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>38474592</t>
+          <t>38402043</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>[['ПП МЕДТОРГ -ЕКСПРЕС', 9], ['ДУ "Волинський обласний центр контролю та профілактики хвороб Міністерства охорони здоров\'я України" (обласний склад)', 7]]</t>
+          <t>[['КП КНП Шепетівський Центр ПМСД', 1], ['КП "КПН Шепетівський Центр ПМСД"', 3], ['КП"КНП Шепетівський ЦентрПМСД', 1], ['КП"КНП Шепетівський Центр ПМСД"', 6], ['КП "КНП Шепетівський Центр ПМСД"', 9], ['КП "КНП Шепетівський Центр ПМСД', 4]]</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>38500472</t>
+          <t>38453281</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>[['КНП "ЦПМСД" Черняхівської селищної ради', 5], ['КНП "ЦПМСД"Черняхівської селищної ради', 6]]</t>
+          <t>[["КНП ''Борзнянський ЦПМСД'' БМР", 5], ["КНП ''Прилуцький міський ЦПМСД''", 2]]</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>38566219</t>
+          <t>38458316</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>[['КНП "Центр ПМСД" КПМР', 10], ['КНП"Центр ПМСД" КПМР', 1]]</t>
+          <t>[['ДУ "Миколаївський ОЦКПХ"', 3], ['ДУ"Миколаївський ОЦКПХ', 6]]</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>38584683</t>
+          <t>38469307</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>[["КНП '' Козелецький ЦПМСД'' КРР", 10], ["КНП ''Сосницький ЦПМСД'' ССР", 1]]</t>
+          <t>[['КНП "Центр ПМД Хмельницького району"', 14], ['КНП "ЦПМД Хмельницького району"', 1], ['КНП"ЦПМД Хмельницького району"', 1]]</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>38584715</t>
+          <t>38474592</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>[["КНП ''Новгород-Сіверський міський ЦПМСД'' Н.-Сіверської МР", 6], ["КНП ''Коропський ЦПМСД'' КСР", 3]]</t>
+          <t>[['ПП МЕДТОРГ -ЕКСПРЕС', 11], ['ДУ "Волинський обласний центр контролю та профілактики хвороб Міністерства охорони здоров\'я України" (обласний склад)', 7]]</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>38611140</t>
+          <t>38476906</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>[['КНП Теофіпольський ЦПСМД', 2], ['КНП "ТЕОФІПОЛЬСЬКИЙ ЦПМСД"', 1], ['Теофіпольський ЦПСМД', 1], ['КНП Теофіпольський ЦПМСД', 3], ['КПН Теофіпольський ЦПМСД', 1]]</t>
+          <t>[['КП "МЦ ПМСД Мішков-Погоріловської с/р"', 7], ['кп"МЦПМСД Мішково-Погорелово', 1]]</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>38822156</t>
+          <t>38487677</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>[['КНП "Березівський міський ЦПМСД"', 11], ['кнп "Березівський міський ЦПМСД"', 1]]</t>
+          <t>[['КНП"Старокостянтинівський ЦПМСД"', 7], ['КНП "Старокостянтинівський ЦПМСД"', 2]]</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>38860558</t>
+          <t>38500472</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>[["КНП '' Лосинівський ЦПМСД'' ЛСР", 18], ["КНП ''Ніжинський міський ЦПМСД'' НМР", 7], ["КНП ''Ічнянський ЦПМСД'' ІМР", 2]]</t>
+          <t>[['КНП "ЦПМСД" Черняхівської селищної ради', 5], ['КНП "ЦПМСД"Черняхівської селищної ради', 6]]</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>39042509</t>
+          <t>38500540</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>[['КНП "Андрушівський ЦПМСД"', 7], ['КНП "ЦПМСД" Андрушівська м/р', 3], ['КНП "ЦПМСД" Андрушівської міської ради', 3]]</t>
+          <t>[['КНП "Чуднівський ЦПМСД" Чуднівської міської ради', 13], ['ТОВ " МЦ Актив-Мед" Любар', 1]]</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>39115875</t>
+          <t>38566219</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>[['ТОВ "КСТ"Фемелі мед клінік"вул. Лізи Чайкіної 69', 8], ['ТОВ "КСТ"Фемелі мед клінік"вул. Лізи Чайкіної 70', 1]]</t>
+          <t>[['КНП "Центр ПМСД" КПМР', 10], ['КНП"Центр ПМСД" КПМР', 1]]</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>39482989</t>
+          <t>38584683</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>[['ТОВ Фастмед Україна', 6], ['ТОВ " Фастмед" України', 1]]</t>
+          <t>[["КНП '' Козелецький ЦПМСД'' КРР", 12], ["КНП ''Сосницький ЦПМСД'' ССР", 1]]</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>40081352</t>
+          <t>38584715</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>[['дніпровська КЛ на залізничному транспорті', 11], ['Львівська клінічна лікарня на залізничному транспорті філії "ЦОЗ" АТ "Укрзалізниця"', 10], ['ХАРКІВСЬКА КЛІНІЧНА ЛІКАРНЯ НА ЗАЛІЗНИЧНОМУ ТРАНСПОРТІ №2 ФІЛІЇ "ЦЕНТР ОХОРОНИ ЗДОРОВ\'Я" АКЦІОНЕРНОГО ТОВАРИСТВА "УКРАЇНСЬКА ЗАЛІЗНИЦЯ"', 2]]</t>
+          <t>[["КНП ''Новгород-Сіверський міський ЦПМСД'' Н.-Сіверської МР", 5], ["КНП ''Коропський ЦПМСД'' КСР", 3]]</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>40208517</t>
+          <t>38611140</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>[['КНП "ЦПМСД Куяльницької сільської ради Подільського району"', 1], ['КНП "ЦПМСД Куяльницької сільської ради Подільського району', 9]]</t>
+          <t>[['КНП Теофіпольський ЦПСМД', 2], ['КНП "ТЕОФІПОЛЬСЬКИЙ ЦПМСД"', 1], ['Теофіпольський ЦПСМД', 1], ['КНП Теофіпольський ЦПМСД', 4], ['КПН Теофіпольський ЦПМСД', 1]]</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>40208847</t>
+          <t>38731750</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>[['КНП ЦПМСД Ушомирської с/р', 5], ['ЦПМСД Ушомирської ср', 6]]</t>
+          <t>[['КНП "ЦПМСД" Радомишльської міської ради', 9], ['КНП "АЗПСМ"Курненської сільської ради', 2], ['Комунальне некомерційне підприємство "Центр первинної медико-санітарної допомоги" Радомишльської міської ради', 1]]</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>40333372</t>
+          <t>38822156</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>[['КНП"ЦПМСД Чорноострівської селищної ради"', 2], ['КНП ЦПМСД Чорний Острів', 1], ['КНП ЦПМСД Чорний ОСТРІВ', 1], ['КНП ЦПМСД ЧорнийОстрів', 2], ['КНП ЦПМСД ЧОРНООСТРІВСЬКОЇ селищної ради', 1]]</t>
+          <t>[['КНП "Березівський міський ЦПМСД"', 12], ['кнп "Березівський міський ЦПМСД"', 1]]</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>40382938</t>
+          <t>38860558</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>[["ТОВ''МЦЗР''100 відсотків життя''", 11], ["ТОВ ''Медичиний центр здоров'я та реабілітації '' 100 відсотків життя''", 3]]</t>
+          <t>[["КНП '' Лосинівський ЦПМСД'' ЛСР", 20], ["КНП ''Ніжинський міський ЦПМСД'' НМР", 8], ["КНП ''Ічнянський ЦПМСД'' ІМР", 2]]</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>40407915</t>
+          <t>39042509</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>[['МЕДКОМ', 10], ['МЕДКОМ Березне', 9]]</t>
+          <t>[['КНП "ЦПМСД" Андрушівська м/р', 6], ['КНП "Андрушівський ЦПМСД"', 6]]</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>40595597</t>
+          <t>40081352</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>[['КНП "ЦПМСД Меджибізької СР"', 4], ['КНП " Меджибізької СР"', 1], ['"КНП ЦПМСД Меджибізької СР"', 1]]</t>
+          <t>[['дніпровська КЛ на залізничному транспорті', 10], ['Львівська клінічна лікарня на залізничному транспорті філії "ЦОЗ" АТ "Укрзалізниця"', 10], ['ХАРКІВСЬКА КЛІНІЧНА ЛІКАРНЯ НА ЗАЛІЗНИЧНОМУ ТРАНСПОРТІ №2 ФІЛІЇ "ЦЕНТР ОХОРОНИ ЗДОРОВ\'Я" АКЦІОНЕРНОГО ТОВАРИСТВА "УКРАЇНСЬКА ЗАЛІЗНИЦЯ"', 2]]</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>41140764</t>
+          <t>40208517</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>[['ТОВ "Приватна поліклініка ПрофіМед"', 8], ['ПП"Приватна поліклініка "Малятко плюс"', 5]]</t>
+          <t>[['КНП "ЦПМСД Куяльницької сільської ради Подільського району"', 1], ['КНП "ЦПМСД Куяльницької сільської ради Подільського району', 9]]</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>41774140</t>
+          <t>40208847</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>[['КП " Медичний лікувально-діагностичний центр " с.Кулевча', 6], ['КП"Медичний лікувально-діагностичний центр" с.Кулевча', 2]]</t>
+          <t>[['ЦПМСД Ушомирської ср', 6], ['КНП ЦПМСД Ушомирської с/р', 5]]</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>41877252</t>
+          <t>40333372</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>[['КНП ЦПМСД Полонської міської ради', 9], ['ІКНП ЦПМСД Полонської міської ради', 1]]</t>
+          <t>[['КНП"ЦПМСД Чорноострівської селищної ради"', 2], ['КНП ЦПМСД Чорний Острів', 1], ['КНП ЦПМСД Чорний ОСТРІВ', 1], ['КНП ЦПМСД ЧорнийОстрів', 2], ['КНП ЦПМСД ЧОРНООСТРІВСЬКОЇ селищної ради', 1]]</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>41931754</t>
+          <t>40358245</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>[['КП "ЦПМСД" Житомирської міської ради', 8], ['КП ЦПМСД ЖМР', 7]]</t>
+          <t>[['ПП "Віва Клінік" м.Славута', 1], ['ПП"Віва Клінік" м.Славута', 1]]</t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>41995294</t>
+          <t>40382938</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>[['КНП "ЦПМСД\' Ямницької сільської ради', 3], ['КНП "ЦПМСД" Ямницької сільської ради', 12]]</t>
+          <t>[["ТОВ''МЦЗР''100 відсотків життя''", 11], ["ТОВ ''Медичиний центр здоров'я та реабілітації '' 100 відсотків життя''", 6]]</t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>42002686</t>
+          <t>40407915</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>[['КНП НМР Центр ПМСД', 11], ['КНП НМР "Центр ПМСД"', 1]]</t>
+          <t>[['МЕДКОМ', 12], ['МЕДКОМ Березне', 8]]</t>
         </is>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>42061427</t>
+          <t>40595597</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>[['КНП "ЦЕНТР ПЕРВИННОЇ МЕДИЧНОЇ ДОПОМОГИ" РОЖНЯТІВСЬКОЇ СЕЛИЩНОЇ РАДИ', 11], ['кнп "ЦЕНТР ПЕРВИННОЇ МЕДИЧНОЇ ДОПОМОГИ" РОЖНЯТІВСЬКОЇ СЕЛИЩНОЇ РАДИ', 1]]</t>
+          <t>[['КНП "ЦПМСД Меджибізької СР"', 4], ['КНП " Меджибізької СР"', 1], ['"КНП ЦПМСД Меджибізької СР"', 1]]</t>
         </is>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>42241755</t>
+          <t>40887956</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>[['КНП «ЦПМСД Березанської міської ради»', 7], ['КНП "Березанський РЦ ПМСД"', 10]]</t>
+          <t>[['КП"ХМЦПМСД №2"', 2], ['КП"ХМЦПМСД№2"', 6], ['ХМЦПМСД№2"', 1]]</t>
         </is>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>42273991</t>
+          <t>40992563</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>[['ТОВ " Медикал Сервіс"', 2], ['Медичний центр ТОВ "Медикал-Сервіс"', 8], ['ТОВ "Медикал сервіс\'\'', 12]]</t>
+          <t>[['КНП"ЦПМСД"Сатанівської селищної ради', 13], ['КНП "ЦПМСД"Сатанівської селищної ради', 1]]</t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>42637772</t>
+          <t>41140764</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>[['КНП «ЦПМСД Березанської міської ради»', 1], ['КНП «Ржищівський міський ЦПМСД» Ржищівської міської ради', 9]]</t>
+          <t>[['ТОВ "Приватна поліклініка ПрофіМед"', 8], ['ПП"Приватна поліклініка "Малятко плюс"', 5]]</t>
         </is>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>43575733</t>
+          <t>41750747</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>[['ТОВ Медична Зірка', 13], ['ТОВ «Медична Зірка»', 9]]</t>
+          <t>[["КНП '' ЦПМСД Наркевицької СР ''", 3], ['КНП " ЦПМСД Наркевицької СР"', 1], ['КНП "ЦПМСД Наркевицької СР"', 4], ['КНП " ЦПМСД Наркевицької СР "', 1]]</t>
         </is>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>43731768</t>
+          <t>41774140</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>[['ТОВ "КСМ"Біхелсі""', 15], ['ТзОВ «КСМ Біхелсі»', 11]]</t>
+          <t>[['КП " Медичний лікувально-діагностичний центр " с.Кулевча', 6], ['КП"Медичний лікувально-діагностичний центр" с.Кулевча', 2]]</t>
         </is>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>43762272</t>
+          <t>41877252</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>[['ТОВ МЦ Лікарська династія', 11], ['ТОВ "Медичний центр "Лікарська династія"', 9]]</t>
+          <t>[['КНП "Полонський ЦПМСД Полонської міської ради"', 1], ['КНП ЦПМСД Полонської міської ради', 9], ['ІКНП ЦПМСД Полонської міської ради', 1]]</t>
         </is>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>43778764</t>
+          <t>41940690</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>[['ТОВ "Медикал плюс"', 3], ['ТзОВ «Медікал плюс»', 5]]</t>
+          <t>[['Комунальне некомерційне підприємство "Довбиський селищний Центр первинної медико-санітарної допомоги"Довбиської селищної ради', 9], ['КНП "Довбиський селищний ЦПМСД"Довбиської селищної ради', 1]]</t>
         </is>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>43858467</t>
+          <t>41995294</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>[['ТОВ "Первинка - 2"', 10], ['ТОВ "МЦ "Первинка-2"', 9]]</t>
+          <t>[['КНП "ЦПМСД\' Ямницької сільської ради', 6], ['КНП "ЦПМСД" Ямницької сільської ради', 10]]</t>
         </is>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>43871190</t>
+          <t>42002686</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>[['ТОВ "Нова Поліклініка Захід"', 10], ['ТОВ «Нова Поліклініка»', 10]]</t>
+          <t>[['КНП НМР Центр ПМСД', 10], ['КНП НМР "Центр ПМСД"', 1]]</t>
         </is>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>44040634</t>
+          <t>42241755</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>[['Комунальне некомерційне підприємство "Амбулаторія загальної практики-сімейної медицини" Барашівської сільської ради', 7], ['КНП «Житомирська багатопрофільна опорна лікарня» Новогуйвинської сел. ради', 2]]</t>
+          <t>[['КНП «ЦПМСД Березанської міської ради»', 9], ['КНП "Березанський РЦ ПМСД"', 15]]</t>
         </is>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>44488596</t>
+          <t>42273991</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>[['КНП "Гульська АЗПСМ"', 5], ['КНП "Гульська АЗПСМ"Стриївської селищної ради', 1]]</t>
+          <t>[['ТОВ "Медикал Сервіс"', 4], ['Медичний центр ТОВ "Медикал-Сервіс"', 8], ['ТОВ "Медикал сервіс\'\'', 12]]</t>
         </is>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
+          <t>42579187</t>
+        </is>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>[['КНП "ЦПМСД" ГУМЕНЕЦЬКОЇ СР', 1], ['КНП "ЦПМСД" Гуменецької СР', 10]]</t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr">
+        <is>
+          <t>43561851</t>
+        </is>
+      </c>
+      <c r="B80" t="inlineStr">
+        <is>
+          <t>[['ТОВ" Перша приватна поліклініка Миколаїв"', 2], ['ТОВ "Перша приватна полклініка Миколаїва"', 19]]</t>
+        </is>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="inlineStr">
+        <is>
+          <t>43575733</t>
+        </is>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>[['ТОВ Медична Зірка', 11], ['ТОВ «Медична Зірка»', 9]]</t>
+        </is>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="inlineStr">
+        <is>
+          <t>43731768</t>
+        </is>
+      </c>
+      <c r="B82" t="inlineStr">
+        <is>
+          <t>[['ТОВ "КСМ"Біхелсі""', 16], ['ТзОВ «КСМ Біхелсі»', 11]]</t>
+        </is>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="inlineStr">
+        <is>
+          <t>43762272</t>
+        </is>
+      </c>
+      <c r="B83" t="inlineStr">
+        <is>
+          <t>[['ТОВ МЦ Лікарська династія', 13], ['ТОВ "Медичний центр "Лікарська династія"', 8]]</t>
+        </is>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="inlineStr">
+        <is>
+          <t>43778764</t>
+        </is>
+      </c>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>[['ТОВ "Медикал плюс"', 3], ['ТзОВ «Медікал плюс»', 5]]</t>
+        </is>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="inlineStr">
+        <is>
+          <t>43858467</t>
+        </is>
+      </c>
+      <c r="B85" t="inlineStr">
+        <is>
+          <t>[['ТОВ "Первинка - 2"', 12], ['ТОВ "МЦ "Первинка-2"', 8]]</t>
+        </is>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="inlineStr">
+        <is>
+          <t>43871190</t>
+        </is>
+      </c>
+      <c r="B86" t="inlineStr">
+        <is>
+          <t>[['ТОВ "Нова Поліклініка Захід"', 12], ['ТОВ «Нова Поліклініка»', 9]]</t>
+        </is>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="inlineStr">
+        <is>
+          <t>44040634</t>
+        </is>
+      </c>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t>[['КНП «Житомирська багатопрофільна опорна лікарня» Новогуйвинської сел. ради', 2], ['Комунальне некомерційне підприємство "Амбулаторія загальної практики-сімейної медицини" Барашівської сільської ради', 5]]</t>
+        </is>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="inlineStr">
+        <is>
           <t>5483121</t>
         </is>
       </c>
-      <c r="B79" t="inlineStr">
+      <c r="B88" t="inlineStr">
         <is>
           <t>[['МДЛ№2', 12], ['MДЛ№2', 1]]</t>
         </is>

</xml_diff>

<commit_message>
Regional and national stock charts are now separated
Vaccine stock forecast now handles future supplies passed through the same datasheet as national stocks

Unified colors for vaccines on the regional chart
</commit_message>
<xml_diff>
--- a/Results/Коди ЄДРПОУ з багатьма варіантами назв закладів.xlsx
+++ b/Results/Коди ЄДРПОУ з багатьма варіантами назв закладів.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B88"/>
+  <dimension ref="A1:B91"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -465,7 +465,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>[['КНП\'\'Тисменицька міська лікарня"Тисменицької міської ради', 14], ['КНП Тисменицька міська лікарня Тисменицької міської ради', 1]]</t>
+          <t>[['КНП\'\'Тисменицька міська лікарня"Тисменицької міської ради', 12], ['КНП Тисменицька міська лікарня Тисменицької міської ради', 1]]</t>
         </is>
       </c>
     </row>
@@ -513,977 +513,1013 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>[['КНП "Городоцька МБЛ" Городоцької міської ради', 1], ['КНП "Городоцька МБЛ"', 1], ['КНП Городоцька МБЛ', 1]]</t>
+          <t>[['КНП "Городоцька МБЛ" Городоцької міської ради', 1], ['КНП "Городоцька МБЛ"', 2]]</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>2004367</t>
+          <t>2004350</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>[['КНА "Летичівська багатопрорфільна лікарня"', 1], ['КРП "Летичівська багатопрофільна лікарня"', 1]]</t>
+          <t>[['КНП"КрасилівськаБЛ"', 1], ['КНП"Красилівська БЛ"', 1]]</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>2004404</t>
+          <t>2004367</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>[['КНП "Полонська МЛ ім. Н. С. Говорун"', 1], ['Комунальне некомерційне підприємство Полонської міської ради "Полонська міська багатопрофільна лікарня ім. Наталії Савеліївни Говорун"', 1]]</t>
+          <t>[['КНА "Летичівська багатопрорфільна лікарня"', 1], ['КРП "Летичівська багатопрофільна лікарня"', 1]]</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>2004812</t>
+          <t>2004404</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>[['КНП "Шепетівська багатопрофільна лікарня" Шепетівської міської ради', 2], ['КНП "Шепетівська багатопофільна лікарня" Шепетівської міської ради', 1], ['КНП"Шепетівська багатопрофільна лікарня" Шепетівської міської ради', 1]]</t>
+          <t>[['КНП "Полонська МЛ ім. Н. С. Говорун"', 2], ['Комунальне некомерційне підприємство Полонської міської ради "Полонська міська багатопрофільна лікарня ім. Наталії Савеліївни Говорун"', 1]]</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>2006194</t>
+          <t>2004746</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>[["КНП ''Коропська ЦЛ'' КСР", 1], ['КНП «Варвинська лікарня» Варвинської селищної ради Прилуцького району Чернігівської області', 1]]</t>
+          <t>[['КП " Хмельницький міський перинатальний центр"', 1], ['КП "Хмельницький міський перинатальний центр"', 2]]</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>2006225</t>
+          <t>2004812</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>[["КНП ''Городнянська МЛ'' ГМР", 16], ["КНП ''Корюківська ЦРЛ'' КМР", 5]]</t>
+          <t>[['КНП "Шепетівська багатопрофільна лікарня" Шепетівської міської ради', 2], ['КНП "Шепетівська багатопофільна лікарня" Шепетівської міської ради', 1], ['КНП"Шепетівська багатопрофільна лікарня" Шепетівської міської ради', 1]]</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>2006604</t>
+          <t>2006194</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>[["КНП ''Сновська ЦРЛ'' СМР", 1], ["КНП ''Прилуцька міська дитяча лікарня'' ПМР", 5]]</t>
+          <t>[["КНП ''Коропська ЦЛ'' КСР", 1], ['КНП «Варвинська лікарня» Варвинської селищної ради Прилуцького району Чернігівської області', 1]]</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>2006610</t>
+          <t>2006225</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>[["КНП ''Чернігівська МЛ №4'' ЧМР", 6], ['КНП «Пологовий будинок» Чернігівської міської ради', 2]]</t>
+          <t>[["КНП ''Городнянська МЛ'' ГМР", 12], ["КНП ''Корюківська ЦРЛ'' КМР", 4]]</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>2007259</t>
+          <t>2006604</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>[['КНП  «КМДЛ №4» КМР» м.Кривий Ріг', 2], ['КП «АМЛ «АМР» м.Апостолове', 1]]</t>
+          <t>[["КНП ''Сновська ЦРЛ'' СМР", 1], ["КНП ''Прилуцька міська дитяча лікарня'' ПМР", 5]]</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>2148517983</t>
+          <t>2006610</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>[['ФОП Олійник Д.Д.', 7], ['ФОП ОЛійник Д.Д.', 1], ['ФОП олійник Д.Д.', 1]]</t>
+          <t>[["КНП ''Чернігівська МЛ №4'' ЧМР", 5], ['КНП «Пологовий будинок» Чернігівської міської ради', 2]]</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>22348948</t>
+          <t>2148517983</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>[['БФ ім. Митрополита А. Шептицького', 6], ['Благодійний Фонд "Шпиталь імені Митрополита Андрея Шептицького Курії Львівської Архиєпархії Української Греко-Католицької Церкви"', 8]]</t>
+          <t>[['ФОП Олійник Д.Д.', 7], ['ФОП ОЛійник Д.Д.', 1], ['ФОП олійник Д.Д.', 1]]</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>2314026147</t>
+          <t>22348948</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>[['ФОП Селезньова С. Л', 4], ['ФОП Селезньова С,Л', 1], ['ФОП Селезньова С.Л', 6]]</t>
+          <t>[['БФ ім. Митрополита А. Шептицького', 6], ['Благодійний Фонд "Шпиталь імені Митрополита Андрея Шептицького Курії Львівської Архиєпархії Української Греко-Католицької Церкви"', 7]]</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>2339913111</t>
+          <t>2314026147</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>[['ФОП "Сем\'янчук В.Б."', 9], ['ФОП Білик Роман Павлович', 10]]</t>
+          <t>[['ФОП Селезньова С. Л', 4], ['ФОП Селезньова С.Л', 4]]</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>26381838</t>
+          <t>2339913111</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>[['КНП " Дитячий МЦ" КПМР', 11], ['КНП " Дитячий МЦ " КПМР', 2]]</t>
+          <t>[['ФОП "Сем\'янчук В.Б."', 9], ['ФОП Білик Роман Павлович', 10]]</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>2727016128</t>
+          <t>2562701239</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>[['ФОП Ковенько Т.', 8], ['ФОП КовенькоТ.', 3]]</t>
+          <t>[['ФОП Маланчик І,А,', 1], ['ФОП "Маланчик"', 5]]</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>2774384</t>
+          <t>26381838</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>[['КП " Хмельницька міська лікарня"', 1], ['КП "Хмльницька міська лікарня"', 1], ['комунальне підприємство "Хмельницька міська лікарня"  Хмельницької міської ради', 1], ['комунальне підприємство "Хмельницька міська лікарня " Хмельницької міської ради', 1]]</t>
+          <t>[['КНП " Дитячий МЦ" КПМР', 11], ['КНП " Дитячий МЦ " КПМР', 2]]</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>2798817680</t>
+          <t>2727016128</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>[['ФОП Слободянюк Л.А.', 43], ['фОП Слободянюк Л.А.', 1], ['ФОП Слободянюк Л.А. педіатр', 86]]</t>
+          <t>[['ФОП Ковенько Т.', 7], ['ФОП КовенькоТ.', 3]]</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>2939705320</t>
+          <t>2774384</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>[['ПП "Віва Клінік"', 4], ['ПП "Віва Клінік" м.Славута', 2], ['ПП " Віва Клінік"', 5]]</t>
+          <t>[['КП " Хмельницька міська лікарня"', 1], ['КП "Хмльницька міська лікарня"', 1], ['комунальне підприємство "Хмельницька міська лікарня"  Хмельницької міської ради', 1], ['комунальне підприємство "Хмельницька міська лікарня " Хмельницької міської ради', 1], ['комунальне підприємство  " Хмельницька міська лікарня" Хмельницької міської ради', 1]]</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>3146414401</t>
+          <t>2798817680</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>[['ФОП Робейко Фаїна Олександрівна', 7], ['ФОП Робейко Фауна Олександрівна', 1]]</t>
+          <t>[['ФОП Слободянюк Л.А.', 43], ['фОП Слободянюк Л.А.', 1], ['ФОП Слободянюк Л.А. педіатр', 102]]</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>3153200965</t>
+          <t>2939705320</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>[['ФОП ГУЗАК ОІ', 7], ['ФОп ГУЗАК ОІ', 1]]</t>
+          <t>[['ПП "Віва Клінік"', 5], ['ПП "Віва Клінік" м.Славута', 2], ['ПП " Віва Клінік"', 5]]</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>3210314064</t>
+          <t>3146414401</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>[['Фоп Осипенко К.В', 3], ['ФОП  Осипенко К.В', 1]]</t>
+          <t>[['ФОП Робейко Фаїна Олександрівна', 7], ['ФОП Робейко Фауна Олександрівна', 1]]</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>3259514282</t>
+          <t>3153200965</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>[['ФОП Віннічук Юлія Валеріївна', 3], ['ФОП Віннічук Ю.В.', 15], ['ФОП ВІннічук Ю.В.', 1]]</t>
+          <t>[['ФОП ГУЗАК ОІ', 6], ['ФОп ГУЗАК ОІ', 1]]</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>3280718060</t>
+          <t>3210314064</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>[['ФОП Гончар Інна Михайлівна', 6], ['Фоп ГоНЧАР ІМ', 1], ['Фоп ГОНЧАР ІМ', 1], ['ФОП ГОНЧАР ІМ', 4]]</t>
+          <t>[['Фоп Осипенко К.В', 3], ['ФОП  Осипенко К.В', 1]]</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>35479197</t>
+          <t>3259514282</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>[['ТОВ Клініка Свій лікар м.Дунаївці', 1], ['ТОВ"КЛІНІКА СВІЙ ЛІКАР"м.Дунаївці', 6], ['ПП"Сіліцея"', 7]]</t>
+          <t>[['ФОП Віннічук Юлія Валеріївна', 3], ['ФОП Віннічук Ю.В.', 20], ['ФОП ВІннічук Ю.В.', 3], ['ФОП ВІНнічук Ю.В.', 1]]</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>37263866</t>
+          <t>3280718060</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>[['ПП"Приватна поліклініка "Малятко плюс"', 45], ['ПП "Малятко плюс"', 25], ['ПП"Малятко плюс"', 2]]</t>
+          <t>[['ФОП Гончар Інна Михайлівна', 6], ['Фоп ГоНЧАР ІМ', 1], ['Фоп ГОНЧАР ІМ', 1], ['ФОП ГОНЧАР ІМ', 4]]</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>37329345</t>
+          <t>35479197</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>[['КНП"СТАРОСИНЯВСЬКИЙ ЦПМСД"', 3], ['КНП СТАРОСИНЯВСЬКИЙ ЦПМСД', 7], ['КНП "СТАРОСИНЯВСЬКИЙ ЦПМСД"', 1]]</t>
+          <t>[['ТОВ Клініка Свій лікар м.Дунаївці', 1], ['ТОВ"КЛІНІКА СВІЙ ЛІКАР"м.Дунаївці', 6], ['ПП"Сіліцея"', 8]]</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>37803420</t>
+          <t>37263866</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>[['КНП "Мирноградський центр первинної медико-санітарної допомоги"', 1], ['КНП "Мирноградський центр первинної медико-санітарної допомоги "', 11], ['КНП " Мирноградський центр первинної медико-санітарної допомоги"', 1]]</t>
+          <t>[['ПП"Приватна поліклініка "Малятко плюс"', 45], ['ПП "Малятко плюс"', 25], ['ПП"Малятко плюс"', 14]]</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>38073028</t>
+          <t>37329345</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>[["КНП ''Городнянський ЦПМСД'' ГМР", 12], ["КНП '' Семенівський ЦПМСД'' СМР", 3]]</t>
+          <t>[['КНП"СТАРОСИНЯВСЬКИЙ ЦПМСД"', 3], ['КНП СТАРОСИНЯВСЬКИЙ ЦПМСД', 7], ['КНП "СТАРОСИНЯВСЬКИЙ ЦПМСД"', 1]]</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>38195551</t>
+          <t>37803420</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>[['КНП "КНП Чемеровецький центр ПМСД"', 1], ['КНП "Чемеровецький центр ПМСД"', 4], ['ТОВ "АЛМ-Поділля"', 3], ['КНП Чемеровецький центр ПМСД', 4]]</t>
+          <t>[['КНП "Мирноградський центр первинної медико-санітарної допомоги"', 1], ['КНП "Мирноградський центр первинної медико-санітарної допомоги "', 10], ['КНП " Мирноградський центр первинної медико-санітарної допомоги"', 1]]</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>38270455</t>
+          <t>38073028</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>[['КНП "Летичівський ЦПМСД"', 6], ['КНП"Летичівський ЦПМСД" Летичівської селищної ради', 2]]</t>
+          <t>[["КНП ''Городнянський ЦПМСД'' ГМР", 13], ["КНП '' Семенівський ЦПМСД'' СМР", 3]]</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>38281797</t>
+          <t>38195551</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>[['КНП"Новоронцовський районний ЦПМСД"', 7], ['КНП"Новоронцовський районний ЦПМСД"(СКЛАД)', 4]]</t>
+          <t>[['КНП "КНП Чемеровецький центр ПМСД"', 1], ['КНП "Чемеровецький центр ПМСД"', 4], ['ТОВ "АЛМ-Поділля"', 3], ['КНП Чемеровецький центр ПМСД', 4]]</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>38283239</t>
+          <t>38270455</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>[['КНП "Ярмолинецький центр ПМСД"', 5], ['КНП "Ярмолинецький центр ПМСД" ЯСР ХО', 1]]</t>
+          <t>[['КНП "Летичівський ЦПМСД"', 8], ['КНП"Летичівський ЦПМСД" Летичівської селищної ради', 2]]</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>38297440</t>
+          <t>38281797</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>[['КНП "Білогірський ЦПМСД"', 6], ['КНП "БІЛОГІРСЬКИЙ ЦПМСД"', 3]]</t>
+          <t>[['КНП"Новоронцовський районний ЦПМСД"', 9], ['КНП"Новоронцовський районний ЦПМСД"(СКЛАД)', 1]]</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>38313933</t>
+          <t>38283239</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>[['КП"Первомайський РЦПМСД', 10], ['КОМУНАЛЬНЕ ПІДПРИЄМСТВО «КАМ’ЯНОПО\xadТОКІВСЬКИЙ ЦЕНТР ПЕРВИННОЇ МЕДИКО-САНІТАРНОЇ ДОПОМОГИ»', 10]]</t>
+          <t>[['КНП "Ярмолинецький центр ПМСД"', 6], ['КНП "Ярмолинецький центр ПМСД" ЯСР ХО', 1]]</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>38341981</t>
+          <t>38297440</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>[['КНП "Бузький РЦ ПСМД"', 8], ['КНП "Бузький РЦ ПМСД"', 1], ['КНП " Бузький ПМСД"', 6]]</t>
+          <t>[['КНП "Білогірський ЦПМСД"', 6], ['КНП "БІЛОГІРСЬКИЙ ЦПМСД"', 4]]</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>38363607</t>
+          <t>38313933</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>[['КНП"Братський ЦПМСД"', 10], ['кнп "Братський ЦПМСД"', 1]]</t>
+          <t>[['КП"Первомайський РЦПМСД', 10], ['КОМУНАЛЬНЕ ПІДПРИЄМСТВО «КАМ’ЯНОПО\xadТОКІВСЬКИЙ ЦЕНТР ПЕРВИННОЇ МЕДИКО-САНІТАРНОЇ ДОПОМОГИ»', 9]]</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>38402043</t>
+          <t>38341981</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>[['КП КНП Шепетівський Центр ПМСД', 1], ['КП "КПН Шепетівський Центр ПМСД"', 3], ['КП"КНП Шепетівський ЦентрПМСД', 1], ['КП"КНП Шепетівський Центр ПМСД"', 6], ['КП "КНП Шепетівський Центр ПМСД"', 9], ['КП "КНП Шепетівський Центр ПМСД', 4]]</t>
+          <t>[['КНП "Бузький РЦ ПСМД"', 8], ['КНП "Бузький РЦ ПМСД"', 1], ['КНП " Бузький ПМСД"', 6]]</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>38453281</t>
+          <t>38363607</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>[["КНП ''Борзнянський ЦПМСД'' БМР", 5], ["КНП ''Прилуцький міський ЦПМСД''", 2]]</t>
+          <t>[['КНП"Братський ЦПМСД"', 10], ['кнп "Братський ЦПМСД"', 1]]</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>38458316</t>
+          <t>38402043</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>[['ДУ "Миколаївський ОЦКПХ"', 3], ['ДУ"Миколаївський ОЦКПХ', 6]]</t>
+          <t>[['КП КНП Шепетівський Центр ПМСД', 1], ['КП "КПН Шепетівський Центр ПМСД"', 3], ['КП"КНП Шепетівський ЦентрПМСД', 2], ['КП"КНП Шепетівський Центр ПМСД"', 6], ['КП "КНП Шепетівський Центр ПМСД"', 7], ['КП "КНП Шепетівський Центр ПМСД', 4]]</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>38469307</t>
+          <t>38453281</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>[['КНП "Центр ПМД Хмельницького району"', 14], ['КНП "ЦПМД Хмельницького району"', 1], ['КНП"ЦПМД Хмельницького району"', 1]]</t>
+          <t>[["КНП ''Борзнянський ЦПМСД'' БМР", 5], ["КНП ''Прилуцький міський ЦПМСД''", 2]]</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>38474592</t>
+          <t>38458316</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>[['ПП МЕДТОРГ -ЕКСПРЕС', 11], ['ДУ "Волинський обласний центр контролю та профілактики хвороб Міністерства охорони здоров\'я України" (обласний склад)', 7]]</t>
+          <t>[['ДУ "Миколаївський ОЦКПХ"', 4], ['ДУ"Миколаївський ОЦКПХ', 6]]</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>38476906</t>
+          <t>38469307</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>[['КП "МЦ ПМСД Мішков-Погоріловської с/р"', 7], ['кп"МЦПМСД Мішково-Погорелово', 1]]</t>
+          <t>[['КНП "Центр ПМД Хмельницького району"', 14], ['КНП "ЦПМД Хмельницького району"', 1], ['КНП"ЦПМД Хмельницького району"', 1]]</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>38487677</t>
+          <t>38474592</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>[['КНП"Старокостянтинівський ЦПМСД"', 7], ['КНП "Старокостянтинівський ЦПМСД"', 2]]</t>
+          <t>[['ПП МЕДТОРГ -ЕКСПРЕС', 11], ['ДУ "Волинський обласний центр контролю та профілактики хвороб Міністерства охорони здоров\'я України" (обласний склад)', 8]]</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>38500472</t>
+          <t>38476906</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>[['КНП "ЦПМСД" Черняхівської селищної ради', 5], ['КНП "ЦПМСД"Черняхівської селищної ради', 6]]</t>
+          <t>[['КП "МЦ ПМСД Мішков-Погоріловської с/р"', 7], ['кп"МЦПМСД Мішково-Погорелово', 1]]</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>38500540</t>
+          <t>38487677</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>[['КНП "Чуднівський ЦПМСД" Чуднівської міської ради', 13], ['ТОВ " МЦ Актив-Мед" Любар', 1]]</t>
+          <t>[['КНП"Старокостянтинівський ЦПМСД"', 6], ['КНП "Старокостянтинівський ЦПМСД"', 3]]</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>38566219</t>
+          <t>38500472</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>[['КНП "Центр ПМСД" КПМР', 10], ['КНП"Центр ПМСД" КПМР', 1]]</t>
+          <t>[['КНП "ЦПМСД" Черняхівської селищної ради', 3], ['КНП "ЦПМСД"Черняхівської селищної ради', 6]]</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>38584683</t>
+          <t>38566219</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>[["КНП '' Козелецький ЦПМСД'' КРР", 12], ["КНП ''Сосницький ЦПМСД'' ССР", 1]]</t>
+          <t>[['КНП "Центр ПМСД" КПМР', 10], ['КНП"Центр ПМСД" КПМР', 1]]</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>38584715</t>
+          <t>38584683</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>[["КНП ''Новгород-Сіверський міський ЦПМСД'' Н.-Сіверської МР", 5], ["КНП ''Коропський ЦПМСД'' КСР", 3]]</t>
+          <t>[["КНП '' Козелецький ЦПМСД'' КРР", 11], ["КНП ''Сосницький ЦПМСД'' ССР", 1]]</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>38611140</t>
+          <t>38584715</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>[['КНП Теофіпольський ЦПСМД', 2], ['КНП "ТЕОФІПОЛЬСЬКИЙ ЦПМСД"', 1], ['Теофіпольський ЦПСМД', 1], ['КНП Теофіпольський ЦПМСД', 4], ['КПН Теофіпольський ЦПМСД', 1]]</t>
+          <t>[["КНП ''Новгород-Сіверський міський ЦПМСД'' Н.-Сіверської МР", 7], ["КНП ''Коропський ЦПМСД'' КСР", 2]]</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>38731750</t>
+          <t>38611140</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>[['КНП "ЦПМСД" Радомишльської міської ради', 9], ['КНП "АЗПСМ"Курненської сільської ради', 2], ['Комунальне некомерційне підприємство "Центр первинної медико-санітарної допомоги" Радомишльської міської ради', 1]]</t>
+          <t>[['КНП Теофіпольський ЦПСМД', 4], ['КНП "ТЕОФІПОЛЬСЬКИЙ ЦПМСД"', 1], ['Теофіпольський ЦПСМД', 1], ['КНП Теофіпольський ЦПМСД', 4], ['КПН Теофіпольський ЦПМСД', 1]]</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>38822156</t>
+          <t>38731750</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>[['КНП "Березівський міський ЦПМСД"', 12], ['кнп "Березівський міський ЦПМСД"', 1]]</t>
+          <t>[['КНП "ЦПМСД" Радомишльської міської ради', 10], ['КНП "АЗПСМ"Курненської сільської ради', 2], ['Комунальне некомерційне підприємство "Центр первинної медико-санітарної допомоги" Радомишльської міської ради', 1]]</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>38860558</t>
+          <t>38822156</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>[["КНП '' Лосинівський ЦПМСД'' ЛСР", 20], ["КНП ''Ніжинський міський ЦПМСД'' НМР", 8], ["КНП ''Ічнянський ЦПМСД'' ІМР", 2]]</t>
+          <t>[['КНП "Березівський міський ЦПМСД"', 12], ['кнп "Березівський міський ЦПМСД"', 1]]</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>39042509</t>
+          <t>38860558</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>[['КНП "ЦПМСД" Андрушівська м/р', 6], ['КНП "Андрушівський ЦПМСД"', 6]]</t>
+          <t>[["КНП '' Лосинівський ЦПМСД'' ЛСР", 20], ["КНП ''Ніжинський міський ЦПМСД'' НМР", 8], ["КНП ''Ічнянський ЦПМСД'' ІМР", 2]]</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>40081352</t>
+          <t>39042509</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>[['дніпровська КЛ на залізничному транспорті', 10], ['Львівська клінічна лікарня на залізничному транспорті філії "ЦОЗ" АТ "Укрзалізниця"', 10], ['ХАРКІВСЬКА КЛІНІЧНА ЛІКАРНЯ НА ЗАЛІЗНИЧНОМУ ТРАНСПОРТІ №2 ФІЛІЇ "ЦЕНТР ОХОРОНИ ЗДОРОВ\'Я" АКЦІОНЕРНОГО ТОВАРИСТВА "УКРАЇНСЬКА ЗАЛІЗНИЦЯ"', 2]]</t>
+          <t>[['КНП "ЦПМСД" Андрушівська м/р', 8], ['КНП "Андрушівський ЦПМСД"', 6]]</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>40208517</t>
+          <t>39089416</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>[['КНП "ЦПМСД Куяльницької сільської ради Подільського району"', 1], ['КНП "ЦПМСД Куяльницької сільської ради Подільського району', 9]]</t>
+          <t>[["КНП ''Сновський ЦПМСД'' СМР", 14], ['КНП «Ічнянська міська лікарня» Ічнянської міської ради', 2]]</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>40208847</t>
+          <t>39115875</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>[['ЦПМСД Ушомирської ср', 6], ['КНП ЦПМСД Ушомирської с/р', 5]]</t>
+          <t>[['ТОВ "КСТ"Фемелі мед клінік"вул. Лізи Чайкіної 69', 6], ['ТОВ "КСТ"Фемелі мед клінік"вул. Лізи Чайкіної 70', 1], ['ТОВ "КСТ"Фемелі мед клінік"вул. Лізи Чайкіної 74', 1]]</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>40333372</t>
+          <t>40081352</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>[['КНП"ЦПМСД Чорноострівської селищної ради"', 2], ['КНП ЦПМСД Чорний Острів', 1], ['КНП ЦПМСД Чорний ОСТРІВ', 1], ['КНП ЦПМСД ЧорнийОстрів', 2], ['КНП ЦПМСД ЧОРНООСТРІВСЬКОЇ селищної ради', 1]]</t>
+          <t>[['дніпровська КЛ на залізничному транспорті', 11], ['Львівська клінічна лікарня на залізничному транспорті філії "ЦОЗ" АТ "Укрзалізниця"', 10], ['ХАРКІВСЬКА КЛІНІЧНА ЛІКАРНЯ НА ЗАЛІЗНИЧНОМУ ТРАНСПОРТІ №2 ФІЛІЇ "ЦЕНТР ОХОРОНИ ЗДОРОВ\'Я" АКЦІОНЕРНОГО ТОВАРИСТВА "УКРАЇНСЬКА ЗАЛІЗНИЦЯ"', 1]]</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>40358245</t>
+          <t>40208847</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>[['ПП "Віва Клінік" м.Славута', 1], ['ПП"Віва Клінік" м.Славута', 1]]</t>
+          <t>[['ЦПМСД Ушомирської ср', 6], ['КНП ЦПМСД Ушомирської с/р', 4]]</t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>40382938</t>
+          <t>40333372</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>[["ТОВ''МЦЗР''100 відсотків життя''", 11], ["ТОВ ''Медичиний центр здоров'я та реабілітації '' 100 відсотків життя''", 6]]</t>
+          <t>[['КНП"ЦПМСД Чорноострівської селищної ради"', 2], ['КНП ЦПМСД Чорноострівської селищної ради', 1], ['КНП ЦПМСД Чорний Острів', 1], ['КНП ЦПМСД Чорний ОСТРІВ', 1], ['КНП ЦПМСД ЧорнийОстрів', 2], ['КНП ЦПМСД ЧОРНООСТРІВСЬКОЇ селищної ради', 1], ["КНП''ЦПМСД ЧОРНИЙ ОСТРІВ''", 1]]</t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>40407915</t>
+          <t>40382938</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>[['МЕДКОМ', 12], ['МЕДКОМ Березне', 8]]</t>
+          <t>[["ТОВ''МЦЗР''100 відсотків життя''", 11], ["ТОВ ''Медичиний центр здоров'я та реабілітації '' 100 відсотків життя''", 6]]</t>
         </is>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>40595597</t>
+          <t>40407915</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>[['КНП "ЦПМСД Меджибізької СР"', 4], ['КНП " Меджибізької СР"', 1], ['"КНП ЦПМСД Меджибізької СР"', 1]]</t>
+          <t>[['МЕДКОМ', 11], ['МЕДКОМ Березне', 7]]</t>
         </is>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>40887956</t>
+          <t>40595597</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>[['КП"ХМЦПМСД №2"', 2], ['КП"ХМЦПМСД№2"', 6], ['ХМЦПМСД№2"', 1]]</t>
+          <t>[['КНП "ЦПМСД Меджибізької СР"', 4], ['КНП " Меджибізької СР"', 1], ['"КНП ЦПМСД Меджибізької СР"', 1]]</t>
         </is>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>40992563</t>
+          <t>40887956</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>[['КНП"ЦПМСД"Сатанівської селищної ради', 13], ['КНП "ЦПМСД"Сатанівської селищної ради', 1]]</t>
+          <t>[['КП"ХМЦПМСД №2"', 2], ['КП"ХМЦПМСД№2"', 6], ['ХМЦПМСД№2"', 1]]</t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>41140764</t>
+          <t>40992563</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>[['ТОВ "Приватна поліклініка ПрофіМед"', 8], ['ПП"Приватна поліклініка "Малятко плюс"', 5]]</t>
+          <t>[['КНП"ЦПМСД"Сатанівської селищної ради', 13], ['КНП "ЦПМСД"Сатанівської селищної ради', 1]]</t>
         </is>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>41750747</t>
+          <t>41140764</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>[["КНП '' ЦПМСД Наркевицької СР ''", 3], ['КНП " ЦПМСД Наркевицької СР"', 1], ['КНП "ЦПМСД Наркевицької СР"', 4], ['КНП " ЦПМСД Наркевицької СР "', 1]]</t>
+          <t>[['ТОВ "Приватна поліклініка ПрофіМед"', 8], ['ПП"Приватна поліклініка "Малятко плюс"', 5]]</t>
         </is>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>41774140</t>
+          <t>41750747</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>[['КП " Медичний лікувально-діагностичний центр " с.Кулевча', 6], ['КП"Медичний лікувально-діагностичний центр" с.Кулевча', 2]]</t>
+          <t>[["КНП '' ЦПМСД Наркевицької СР ''", 3], ['КНП " ЦПМСД Наркевицької СР"', 1], ['КНП "ЦПМСД Наркевицької СР"', 4], ['КНП " ЦПМСД Наркевицької СР "', 1]]</t>
         </is>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>41877252</t>
+          <t>41774140</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>[['КНП "Полонський ЦПМСД Полонської міської ради"', 1], ['КНП ЦПМСД Полонської міської ради', 9], ['ІКНП ЦПМСД Полонської міської ради', 1]]</t>
+          <t>[['КП " Медичний лікувально-діагностичний центр " с.Кулевча', 6], ['КП"Медичний лікувально-діагностичний центр" с.Кулевча', 2], ['КП"Медичний лікувально-діагностичний центр"', 1]]</t>
         </is>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>41940690</t>
+          <t>41877252</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>[['Комунальне некомерційне підприємство "Довбиський селищний Центр первинної медико-санітарної допомоги"Довбиської селищної ради', 9], ['КНП "Довбиський селищний ЦПМСД"Довбиської селищної ради', 1]]</t>
+          <t>[['КНП ЦПМСД Полонської міської ради', 10], ['ІКНП ЦПМСД Полонської міської ради', 1]]</t>
         </is>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>41995294</t>
+          <t>41940690</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>[['КНП "ЦПМСД\' Ямницької сільської ради', 6], ['КНП "ЦПМСД" Ямницької сільської ради', 10]]</t>
+          <t>[['Комунальне некомерційне підприємство "Довбиський селищний Центр первинної медико-санітарної допомоги"Довбиської селищної ради', 9], ['КНП "Довбиський селищний ЦПМСД"Довбиської селищної ради', 1]]</t>
         </is>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>42002686</t>
+          <t>41995294</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>[['КНП НМР Центр ПМСД', 10], ['КНП НМР "Центр ПМСД"', 1]]</t>
+          <t>[['КНП "ЦПМСД\' Ямницької сільської ради', 6], ['КНП "ЦПМСД" Ямницької сільської ради', 9]]</t>
         </is>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>42241755</t>
+          <t>42002686</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>[['КНП «ЦПМСД Березанської міської ради»', 9], ['КНП "Березанський РЦ ПМСД"', 15]]</t>
+          <t>[['КНП НМР Центр ПМСД', 10], ['КНП НМР "Центр ПМСД"', 1]]</t>
         </is>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>42273991</t>
+          <t>42241755</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>[['ТОВ "Медикал Сервіс"', 4], ['Медичний центр ТОВ "Медикал-Сервіс"', 8], ['ТОВ "Медикал сервіс\'\'', 12]]</t>
+          <t>[['КНП «ЦПМСД Березанської міської ради»', 8], ['КНП "Березанський РЦ ПМСД"', 15]]</t>
         </is>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>42579187</t>
+          <t>42273991</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>[['КНП "ЦПМСД" ГУМЕНЕЦЬКОЇ СР', 1], ['КНП "ЦПМСД" Гуменецької СР', 10]]</t>
+          <t>[['ТОВ " Медикал Сервіс"', 5], ['Медичний центр ТОВ "Медикал-Сервіс"', 8], ['ТОВ "Медикал сервіс\'\'', 12]]</t>
         </is>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>43561851</t>
+          <t>42277419</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>[['ТОВ" Перша приватна поліклініка Миколаїв"', 2], ['ТОВ "Перша приватна полклініка Миколаїва"', 19]]</t>
+          <t>[['КНП "Шепетівський міський центр ПМСД" Шепетівської ради', 5], ['КНП Шепетівський МЦ ПМСД', 1]]</t>
         </is>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>43575733</t>
+          <t>42500117</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>[['ТОВ Медична Зірка', 11], ['ТОВ «Медична Зірка»', 9]]</t>
+          <t>[['КНП "Центр первинної медико-санітарної допомоги" Южненської міської ради', 5], ['кНП "Центр первинної медико-санітарної допомоги" Южненської міської ради', 1]]</t>
         </is>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>43731768</t>
+          <t>42579187</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>[['ТОВ "КСМ"Біхелсі""', 16], ['ТзОВ «КСМ Біхелсі»', 11]]</t>
+          <t>[['КНП "ЦПМСД" ГУМЕНЕЦЬКОЇ СР', 1], ['КНП "ЦПМСД" Гуменецької СР', 12]]</t>
         </is>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>43762272</t>
+          <t>43561851</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>[['ТОВ МЦ Лікарська династія', 13], ['ТОВ "Медичний центр "Лікарська династія"', 8]]</t>
+          <t>[['ТОВ" Перша приватна поліклініка Миколаїв"', 2], ['ТОВ "Перша приватна полклініка Миколаїва"', 19]]</t>
         </is>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>43778764</t>
+          <t>43575733</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>[['ТОВ "Медикал плюс"', 3], ['ТзОВ «Медікал плюс»', 5]]</t>
+          <t>[['ТОВ Медична Зірка', 12], ['ТОВ «Медична Зірка»', 9]]</t>
         </is>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>43858467</t>
+          <t>43731768</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>[['ТОВ "Первинка - 2"', 12], ['ТОВ "МЦ "Первинка-2"', 8]]</t>
+          <t>[['ТОВ "КСМ"Біхелсі""', 16], ['ТзОВ «КСМ Біхелсі»', 11]]</t>
         </is>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>43871190</t>
+          <t>43762272</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>[['ТОВ "Нова Поліклініка Захід"', 12], ['ТОВ «Нова Поліклініка»', 9]]</t>
+          <t>[['ТОВ МЦ Лікарська династія', 13], ['ТОВ "Медичний центр "Лікарська династія"', 10]]</t>
         </is>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>44040634</t>
+          <t>43778764</t>
         </is>
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>[['КНП «Житомирська багатопрофільна опорна лікарня» Новогуйвинської сел. ради', 2], ['Комунальне некомерційне підприємство "Амбулаторія загальної практики-сімейної медицини" Барашівської сільської ради', 5]]</t>
+          <t>[['ТОВ "Медикал плюс"', 4], ['ТзОВ «Медікал плюс»', 5]]</t>
         </is>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
+          <t>43858467</t>
+        </is>
+      </c>
+      <c r="B88" t="inlineStr">
+        <is>
+          <t>[['ТОВ "Первинка - 2"', 13], ['ТОВ "МЦ "Первинка-2"', 8]]</t>
+        </is>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="inlineStr">
+        <is>
+          <t>43871190</t>
+        </is>
+      </c>
+      <c r="B89" t="inlineStr">
+        <is>
+          <t>[['ТОВ "Нова Поліклініка Захід"', 12], ['ТОВ «Нова Поліклініка»', 9]]</t>
+        </is>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="inlineStr">
+        <is>
+          <t>44040634</t>
+        </is>
+      </c>
+      <c r="B90" t="inlineStr">
+        <is>
+          <t>[['КНП «Житомирська багатопрофільна опорна лікарня» Новогуйвинської сел. ради', 2], ['Комунальне некомерційне підприємство "Амбулаторія загальної практики-сімейної медицини" Барашівської сільської ради', 5]]</t>
+        </is>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="inlineStr">
+        <is>
           <t>5483121</t>
         </is>
       </c>
-      <c r="B88" t="inlineStr">
+      <c r="B91" t="inlineStr">
         <is>
           <t>[['МДЛ№2', 12], ['MДЛ№2', 1]]</t>
         </is>

</xml_diff>

<commit_message>
15.03.2024 Update and bug fixes
</commit_message>
<xml_diff>
--- a/Results/Коди ЄДРПОУ з багатьма варіантами назв закладів.xlsx
+++ b/Results/Коди ЄДРПОУ з багатьма варіантами назв закладів.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B91"/>
+  <dimension ref="A1:B93"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -448,240 +448,240 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>1990756</t>
+          <t>14280960</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>[['КНП"БЛІЛ КМР"', 5], ['КНП"БЛІЛ КМР', 1]]</t>
+          <t>[['КНП"ЖовтоводськаМЛ"', 3], ['КНП"Жовтоводська МЛ"ЖМР', 1]]</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>1993486</t>
+          <t>1983814</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>[['КНП\'\'Тисменицька міська лікарня"Тисменицької міської ради', 12], ['КНП Тисменицька міська лікарня Тисменицької міської ради', 1]]</t>
+          <t>[['КНП"Херсонська міська клінична лікарня ім.Карабелеша"', 14], ['КНП"Новоронцовський районний ЦПМСД"', 1]]</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>1995290</t>
+          <t>1990756</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>[['КНП "Петрівська Центральна лікарня" Петрівської селищної ради', 1], ['КНП "Петрівська Центральна лікарня" Петрівської районної ради', 1]]</t>
+          <t>[['КНП"БЛІЛ КМР"', 5], ['КНП"БЛІЛ КМР', 1]]</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>1998354</t>
+          <t>1993486</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>[['КНП "Баштанська БПЛ"', 3], ['КНП"Баштанська БПЛ', 4]]</t>
+          <t>[['КНП\'\'Тисменицька міська лікарня"Тисменицької міської ради', 12], ['КНП Тисменицька міська лікарня Тисменицької міської ради', 1]]</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>1998785</t>
+          <t>1995290</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>[['КНП "Кодимська лікарня" Кодимської міської ради Подільського району Одеської області', 2], ['КНП "Кодимська лікарня"\n  Кодимської міської ради\n  Подільського району\n  Одеської області', 2]]</t>
+          <t>[['КНП "Петрівська Центральна лікарня" Петрівської селищної ради', 1], ['КНП "Петрівська Центральна лікарня" Петрівської районної ради', 1]]</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>2004216</t>
+          <t>1998785</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>[['КНП "Городоцька МБЛ" Городоцької міської ради', 1], ['КНП "Городоцька МБЛ"', 2]]</t>
+          <t>[['КНП "Кодимська лікарня" Кодимської міської ради Подільського району Одеської області', 2], ['КНП "Кодимська лікарня"\n  Кодимської міської ради\n  Подільського району\n  Одеської області', 2]]</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>2004350</t>
+          <t>2004216</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>[['КНП"КрасилівськаБЛ"', 1], ['КНП"Красилівська БЛ"', 1]]</t>
+          <t>[['КНП "Городоцька МБЛ" Городоцької міської ради', 1], ['КНП "Городоцька МБЛ"', 2]]</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>2004367</t>
+          <t>2004350</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>[['КНА "Летичівська багатопрорфільна лікарня"', 1], ['КРП "Летичівська багатопрофільна лікарня"', 1]]</t>
+          <t>[['КНП"КрасилівськаБЛ"', 1], ['КНП "Красилівська БЛ"', 1], ['КНП"Красилівська БЛ"', 1]]</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>2004404</t>
+          <t>2004367</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>[['КНП "Полонська МЛ ім. Н. С. Говорун"', 2], ['Комунальне некомерційне підприємство Полонської міської ради "Полонська міська багатопрофільна лікарня ім. Наталії Савеліївни Говорун"', 1]]</t>
+          <t>[['КНА "Летичівська багатопрорфільна лікарня"', 1], ['КРП "Летичівська багатопрофільна лікарня"', 1]]</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>2004746</t>
+          <t>2004404</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>[['КП " Хмельницький міський перинатальний центр"', 1], ['КП "Хмельницький міський перинатальний центр"', 2]]</t>
+          <t>[['КНП "Полонська МЛ ім. Н. С. Говорун"', 2], ['Комунальне некомерційне підприємство Полонської міської ради "Полонська міська багатопрофільна лікарня ім. Наталії Савеліївни Говорун"', 1]]</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>2004812</t>
+          <t>2004746</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>[['КНП "Шепетівська багатопрофільна лікарня" Шепетівської міської ради', 2], ['КНП "Шепетівська багатопофільна лікарня" Шепетівської міської ради', 1], ['КНП"Шепетівська багатопрофільна лікарня" Шепетівської міської ради', 1]]</t>
+          <t>[['КП " Хмельницький міський перинатальний центр"', 1], ['КП "Хмельницький міський перинатальний центр"', 2]]</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>2006194</t>
+          <t>2004812</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>[["КНП ''Коропська ЦЛ'' КСР", 1], ['КНП «Варвинська лікарня» Варвинської селищної ради Прилуцького району Чернігівської області', 1]]</t>
+          <t>[['КНП "Шепетівська багатопрофільна лікарня" Шепетівської міської ради', 2], ['КНП "Шепетівська багатопофільна лікарня" Шепетівської міської ради', 1], ['КНП"Шепетівська багатопрофільна лікарня" Шепетівської міської ради', 1]]</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>2006225</t>
+          <t>2006194</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>[["КНП ''Городнянська МЛ'' ГМР", 12], ["КНП ''Корюківська ЦРЛ'' КМР", 4]]</t>
+          <t>[["КНП ''Коропська ЦЛ'' КСР", 1], ['КНП «Варвинська лікарня» Варвинської селищної ради Прилуцького району Чернігівської області', 1]]</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>2006604</t>
+          <t>2006225</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>[["КНП ''Сновська ЦРЛ'' СМР", 1], ["КНП ''Прилуцька міська дитяча лікарня'' ПМР", 5]]</t>
+          <t>[["КНП ''Городнянська МЛ'' ГМР", 12], ["КНП ''Корюківська ЦРЛ'' КМР", 4]]</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>2006610</t>
+          <t>2006604</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>[["КНП ''Чернігівська МЛ №4'' ЧМР", 5], ['КНП «Пологовий будинок» Чернігівської міської ради', 2]]</t>
+          <t>[["КНП ''Сновська ЦРЛ'' СМР", 1], ["КНП ''Прилуцька міська дитяча лікарня'' ПМР", 5]]</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>2148517983</t>
+          <t>2006610</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>[['ФОП Олійник Д.Д.', 7], ['ФОП ОЛійник Д.Д.', 1], ['ФОП олійник Д.Д.', 1]]</t>
+          <t>[["КНП ''Чернігівська МЛ №4'' ЧМР", 5], ['КНП «Пологовий будинок» Чернігівської міської ради', 2]]</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>22348948</t>
+          <t>2148517983</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>[['БФ ім. Митрополита А. Шептицького', 6], ['Благодійний Фонд "Шпиталь імені Митрополита Андрея Шептицького Курії Львівської Архиєпархії Української Греко-Католицької Церкви"', 7]]</t>
+          <t>[['ФОП Олійник Д.Д.', 8], ['ФОП ОЛійник Д.Д.', 1], ['ФОП олійник Д.Д.', 1]]</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>2314026147</t>
+          <t>22348948</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>[['ФОП Селезньова С. Л', 4], ['ФОП Селезньова С.Л', 4]]</t>
+          <t>[['БФ ім. Митрополита А. Шептицького', 6], ['Благодійний Фонд "Шпиталь імені Митрополита Андрея Шептицького Курії Львівської Архиєпархії Української Греко-Католицької Церкви"', 12]]</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>2339913111</t>
+          <t>2314026147</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>[['ФОП "Сем\'янчук В.Б."', 9], ['ФОП Білик Роман Павлович', 10]]</t>
+          <t>[['ФОП Селезньова С. Л', 3], ['ФОП Селезньова С.Л', 3]]</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>2562701239</t>
+          <t>2339913111</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>[['ФОП Маланчик І,А,', 1], ['ФОП "Маланчик"', 5]]</t>
+          <t>[['ФОП "Сем\'янчук В.Б."', 9], ['ФОП Білик Роман Павлович', 10]]</t>
         </is>
       </c>
     </row>
@@ -693,7 +693,7 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>[['КНП " Дитячий МЦ" КПМР', 11], ['КНП " Дитячий МЦ " КПМР', 2]]</t>
+          <t>[['КНП " Дитячий МЦ" КПМР', 10], ['КНП " Дитячий МЦ " КПМР', 2]]</t>
         </is>
       </c>
     </row>
@@ -705,7 +705,7 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>[['ФОП Ковенько Т.', 7], ['ФОП КовенькоТ.', 3]]</t>
+          <t>[['ФОП Ковенько Т.', 8], ['ФОП КовенькоТ.', 3]]</t>
         </is>
       </c>
     </row>
@@ -717,7 +717,7 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>[['КП " Хмельницька міська лікарня"', 1], ['КП "Хмльницька міська лікарня"', 1], ['комунальне підприємство "Хмельницька міська лікарня"  Хмельницької міської ради', 1], ['комунальне підприємство "Хмельницька міська лікарня " Хмельницької міської ради', 1], ['комунальне підприємство  " Хмельницька міська лікарня" Хмельницької міської ради', 1]]</t>
+          <t>[['КП " Хмельницька міська лікарня"', 1], ['КП "Хмльницька міська лікарня"', 1], ['комунальне підприємство "Хмельницька міська лікарня " Хмельницької міської ради', 1], ['комунальне підприємство  " Хмельницька міська лікарня" Хмельницької міської ради', 1]]</t>
         </is>
       </c>
     </row>
@@ -729,7 +729,7 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>[['ФОП Слободянюк Л.А.', 43], ['фОП Слободянюк Л.А.', 1], ['ФОП Слободянюк Л.А. педіатр', 102]]</t>
+          <t>[['ФОП Слободянюк Л.А.', 43], ['фОП Слободянюк Л.А.', 1], ['ФОП Слободянюк Л.А. педіатр', 110]]</t>
         </is>
       </c>
     </row>
@@ -748,778 +748,802 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>3146414401</t>
+          <t>2975100945</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>[['ФОП Робейко Фаїна Олександрівна', 7], ['ФОП Робейко Фауна Олександрівна', 1]]</t>
+          <t>[['ФОП Ковтун Людмила Володимирівна', 11], ['фОП Ковтун Людмила Володимирівна', 1]]</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>3153200965</t>
+          <t>3146414401</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>[['ФОП ГУЗАК ОІ', 6], ['ФОп ГУЗАК ОІ', 1]]</t>
+          <t>[['ФОП Робейко Фаїна Олександрівна', 7], ['ФОП Робейко Фауна Олександрівна', 1]]</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>3210314064</t>
+          <t>3153200965</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>[['Фоп Осипенко К.В', 3], ['ФОП  Осипенко К.В', 1]]</t>
+          <t>[['ФОП ГУЗАК ОІ', 6], ['ФОп ГУЗАК ОІ', 1]]</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>3259514282</t>
+          <t>3210314064</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>[['ФОП Віннічук Юлія Валеріївна', 3], ['ФОП Віннічук Ю.В.', 20], ['ФОП ВІннічук Ю.В.', 3], ['ФОП ВІНнічук Ю.В.', 1]]</t>
+          <t>[['Фоп Осипенко К.В', 3], ['ФОП  Осипенко К.В', 1]]</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>3280718060</t>
+          <t>3259514282</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>[['ФОП Гончар Інна Михайлівна', 6], ['Фоп ГоНЧАР ІМ', 1], ['Фоп ГОНЧАР ІМ', 1], ['ФОП ГОНЧАР ІМ', 4]]</t>
+          <t>[['ФОП Віннічук Юлія Валеріївна', 3], ['ФОП Віннічук Ю.В.', 20], ['ФОП ВІннічук Ю.В.', 3], ['ФОП ВІНнічук Ю.В.', 1]]</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>35479197</t>
+          <t>3280718060</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>[['ТОВ Клініка Свій лікар м.Дунаївці', 1], ['ТОВ"КЛІНІКА СВІЙ ЛІКАР"м.Дунаївці', 6], ['ПП"Сіліцея"', 8]]</t>
+          <t>[['ФОП Гончар Інна Михайлівна', 6], ['Фоп ГоНЧАР ІМ', 1], ['Фоп ГОНЧАР ІМ', 1], ['ФОП ГОНЧАР ІМ', 4]]</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>37263866</t>
+          <t>35479197</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>[['ПП"Приватна поліклініка "Малятко плюс"', 45], ['ПП "Малятко плюс"', 25], ['ПП"Малятко плюс"', 14]]</t>
+          <t>[['ТОВ Клініка Свій лікар м.Дунаївці', 1], ['ТОВ"КЛІНІКА СВІЙ ЛІКАР"м.Дунаївці', 6], ['ПП"Сіліцея"', 7]]</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>37329345</t>
+          <t>37263866</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>[['КНП"СТАРОСИНЯВСЬКИЙ ЦПМСД"', 3], ['КНП СТАРОСИНЯВСЬКИЙ ЦПМСД', 7], ['КНП "СТАРОСИНЯВСЬКИЙ ЦПМСД"', 1]]</t>
+          <t>[['ПП"Приватна поліклініка "Малятко плюс"', 45], ['ПП "Малятко плюс"', 25], ['ПП"Малятко плюс"', 20]]</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>37803420</t>
+          <t>37329345</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>[['КНП "Мирноградський центр первинної медико-санітарної допомоги"', 1], ['КНП "Мирноградський центр первинної медико-санітарної допомоги "', 10], ['КНП " Мирноградський центр первинної медико-санітарної допомоги"', 1]]</t>
+          <t>[['КНП"СТАРОСИНЯВСЬКИЙ ЦПМСД"', 3], ['КНП СТАРОСИНЯВСЬКИЙ ЦПМСД', 7], ['КНП "СТАРОСИНЯВСЬКИЙ ЦПМСД"', 1]]</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>38073028</t>
+          <t>37803420</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>[["КНП ''Городнянський ЦПМСД'' ГМР", 13], ["КНП '' Семенівський ЦПМСД'' СМР", 3]]</t>
+          <t>[['КНП "Мирноградський центр первинної медико-санітарної допомоги"', 1], ['КНП "Мирноградський центр первинної медико-санітарної допомоги "', 10], ['КНП " Мирноградський центр первинної медико-санітарної допомоги"', 1]]</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>38195551</t>
+          <t>38073028</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>[['КНП "КНП Чемеровецький центр ПМСД"', 1], ['КНП "Чемеровецький центр ПМСД"', 4], ['ТОВ "АЛМ-Поділля"', 3], ['КНП Чемеровецький центр ПМСД', 4]]</t>
+          <t>[["КНП ''Городнянський ЦПМСД'' ГМР", 13], ["КНП '' Семенівський ЦПМСД'' СМР", 3]]</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>38270455</t>
+          <t>38195242</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>[['КНП "Летичівський ЦПМСД"', 8], ['КНП"Летичівський ЦПМСД" Летичівської селищної ради', 2]]</t>
+          <t>[['КНП «Деражнянський ЦПМСД» ДМР ХО', 9], ['КПН "Деражнянський ЦПМСД"ДМР ХО', 1]]</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>38281797</t>
+          <t>38195551</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>[['КНП"Новоронцовський районний ЦПМСД"', 9], ['КНП"Новоронцовський районний ЦПМСД"(СКЛАД)', 1]]</t>
+          <t>[['КНП "КНП Чемеровецький центр ПМСД"', 1], ['КНП "Чемеровецький центр ПМСД"', 6], ['ТОВ "АЛМ-Поділля"', 3], ['КНП Чемеровецький центр ПМСД', 4]]</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>38283239</t>
+          <t>38270455</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>[['КНП "Ярмолинецький центр ПМСД"', 6], ['КНП "Ярмолинецький центр ПМСД" ЯСР ХО', 1]]</t>
+          <t>[['КНП "Летичівський ЦПМСД"', 8], ['КНП"Летичівський ЦПМСД" Летичівської селищної ради', 2]]</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>38297440</t>
+          <t>38281797</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>[['КНП "Білогірський ЦПМСД"', 6], ['КНП "БІЛОГІРСЬКИЙ ЦПМСД"', 4]]</t>
+          <t>[['КНП"Новоронцовський районний ЦПМСД"', 10], ['КНП"Новоронцовський районний ЦПМСД"(СКЛАД)', 1]]</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>38313933</t>
+          <t>38283239</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>[['КП"Первомайський РЦПМСД', 10], ['КОМУНАЛЬНЕ ПІДПРИЄМСТВО «КАМ’ЯНОПО\xadТОКІВСЬКИЙ ЦЕНТР ПЕРВИННОЇ МЕДИКО-САНІТАРНОЇ ДОПОМОГИ»', 9]]</t>
+          <t>[['КНП "Ярмолинецький центр ПМСД"', 6], ['КНП "Ярмолинецький центр ПМСД" ЯСР ХО', 1]]</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>38341981</t>
+          <t>38297440</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>[['КНП "Бузький РЦ ПСМД"', 8], ['КНП "Бузький РЦ ПМСД"', 1], ['КНП " Бузький ПМСД"', 6]]</t>
+          <t>[['КНП "Білогірський ЦПМСД"', 6], ['КНП "БІЛОГІРСЬКИЙ ЦПМСД"', 4]]</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>38363607</t>
+          <t>38313933</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>[['КНП"Братський ЦПМСД"', 10], ['кнп "Братський ЦПМСД"', 1]]</t>
+          <t>[['КП"Первомайський РЦПМСД', 10], ['КОМУНАЛЬНЕ ПІДПРИЄМСТВО «КАМ’ЯНОПО\xadТОКІВСЬКИЙ ЦЕНТР ПЕРВИННОЇ МЕДИКО-САНІТАРНОЇ ДОПОМОГИ»', 9]]</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>38402043</t>
+          <t>38331800</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>[['КП КНП Шепетівський Центр ПМСД', 1], ['КП "КПН Шепетівський Центр ПМСД"', 3], ['КП"КНП Шепетівський ЦентрПМСД', 2], ['КП"КНП Шепетівський Центр ПМСД"', 6], ['КП "КНП Шепетівський Центр ПМСД"', 7], ['КП "КНП Шепетівський Центр ПМСД', 4]]</t>
+          <t>[['ДУ Івано-Франківський ОЦКПХ', 11], ['Снятинський відділ', 8]]</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>38453281</t>
+          <t>38341981</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>[["КНП ''Борзнянський ЦПМСД'' БМР", 5], ["КНП ''Прилуцький міський ЦПМСД''", 2]]</t>
+          <t>[['КНП "Бузький РЦ ПСМД"', 8], ['КНП "Бузький РЦ ПМСД"', 1], ['КНП " Бузький ПМСД"', 6]]</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>38458316</t>
+          <t>38363607</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>[['ДУ "Миколаївський ОЦКПХ"', 4], ['ДУ"Миколаївський ОЦКПХ', 6]]</t>
+          <t>[['КНП"Братський ЦПМСД"', 10], ['кнп "Братський ЦПМСД"', 1]]</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>38469307</t>
+          <t>38402043</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>[['КНП "Центр ПМД Хмельницького району"', 14], ['КНП "ЦПМД Хмельницького району"', 1], ['КНП"ЦПМД Хмельницького району"', 1]]</t>
+          <t>[['КП КНП Шепетівський Центр ПМСД', 1], ['КП "КПН Шепетівський Центр ПМСД"', 3], ['КП"КНП Шепетівський ЦентрПМСД', 2], ['КП"КНП Шепетівський Центр ПМСД"', 6], ['КП "КНП Шепетівський Центр ПМСД"', 7], ['КП "КНП Шепетівський Центр ПМСД', 4]]</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>38474592</t>
+          <t>38453281</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>[['ПП МЕДТОРГ -ЕКСПРЕС', 11], ['ДУ "Волинський обласний центр контролю та профілактики хвороб Міністерства охорони здоров\'я України" (обласний склад)', 8]]</t>
+          <t>[["КНП ''Борзнянський ЦПМСД'' БМР", 5], ["КНП ''Прилуцький міський ЦПМСД''", 2]]</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>38476906</t>
+          <t>38458316</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>[['КП "МЦ ПМСД Мішков-Погоріловської с/р"', 7], ['кп"МЦПМСД Мішково-Погорелово', 1]]</t>
+          <t>[['ДУ "Миколаївський ОЦКПХ"', 4], ['ДУ"Миколаївський ОЦКПХ', 6]]</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>38487677</t>
+          <t>38469307</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>[['КНП"Старокостянтинівський ЦПМСД"', 6], ['КНП "Старокостянтинівський ЦПМСД"', 3]]</t>
+          <t>[['КНП "Центр ПМД Хмельницького району"', 12], ['КНП "ЦПМД Хмельницького району"', 1]]</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>38500472</t>
+          <t>38474592</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>[['КНП "ЦПМСД" Черняхівської селищної ради', 3], ['КНП "ЦПМСД"Черняхівської селищної ради', 6]]</t>
+          <t>[['ПП МЕДТОРГ -ЕКСПРЕС', 10], ['ДУ "Волинський обласний центр контролю та профілактики хвороб Міністерства охорони здоров\'я України" (обласний склад)', 6]]</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>38566219</t>
+          <t>38487677</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>[['КНП "Центр ПМСД" КПМР', 10], ['КНП"Центр ПМСД" КПМР', 1]]</t>
+          <t>[['КНП"Старокостянтинівський ЦПМСД"', 6], ['КНП "Старокостянтинівський ЦПМСД"', 3]]</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>38584683</t>
+          <t>38500472</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>[["КНП '' Козелецький ЦПМСД'' КРР", 11], ["КНП ''Сосницький ЦПМСД'' ССР", 1]]</t>
+          <t>[['КНП "ЦПМСД" Черняхівської селищної ради', 4], ['КНП "ЦПМСД"Черняхівської селищної ради', 7]]</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>38584715</t>
+          <t>38566219</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>[["КНП ''Новгород-Сіверський міський ЦПМСД'' Н.-Сіверської МР", 7], ["КНП ''Коропський ЦПМСД'' КСР", 2]]</t>
+          <t>[['КНП "Центр ПМСД" КПМР', 10], ['КНП"Центр ПМСД" КПМР', 1]]</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>38611140</t>
+          <t>38584683</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>[['КНП Теофіпольський ЦПСМД', 4], ['КНП "ТЕОФІПОЛЬСЬКИЙ ЦПМСД"', 1], ['Теофіпольський ЦПСМД', 1], ['КНП Теофіпольський ЦПМСД', 4], ['КПН Теофіпольський ЦПМСД', 1]]</t>
+          <t>[["КНП '' Козелецький ЦПМСД'' КРР", 10], ["КНП ''Сосницький ЦПМСД'' ССР", 1]]</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>38731750</t>
+          <t>38584715</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>[['КНП "ЦПМСД" Радомишльської міської ради', 10], ['КНП "АЗПСМ"Курненської сільської ради', 2], ['Комунальне некомерційне підприємство "Центр первинної медико-санітарної допомоги" Радомишльської міської ради', 1]]</t>
+          <t>[["КНП ''Новгород-Сіверський міський ЦПМСД'' Н.-Сіверської МР", 7], ["КНП ''Коропський ЦПМСД'' КСР", 1]]</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>38822156</t>
+          <t>38611140</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>[['КНП "Березівський міський ЦПМСД"', 12], ['кнп "Березівський міський ЦПМСД"', 1]]</t>
+          <t>[['КНП Теофіпольський ЦПСМД', 4], ['КНП "ТЕОФІПОЛЬСЬКИЙ ЦПМСД"', 1], ['Теофіпольський ЦПСМД', 1], ['КНП Теофіпольський ЦПМСД', 4], ['КПН Теофіпольський ЦПМСД', 1]]</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>38860558</t>
+          <t>38731750</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>[["КНП '' Лосинівський ЦПМСД'' ЛСР", 20], ["КНП ''Ніжинський міський ЦПМСД'' НМР", 8], ["КНП ''Ічнянський ЦПМСД'' ІМР", 2]]</t>
+          <t>[['КНП "ЦПМСД" Радомишльської міської ради', 10], ['КНП "АЗПСМ"Курненської сільської ради', 2], ['Комунальне некомерційне підприємство "Центр первинної медико-санітарної допомоги" Радомишльської міської ради', 2]]</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>39042509</t>
+          <t>38809093</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>[['КНП "ЦПМСД" Андрушівська м/р', 8], ['КНП "Андрушівський ЦПМСД"', 6]]</t>
+          <t>[['КНП "Вільнянський ЦПМСД"ВМР', 18], ['КНП "Вільнянський ЦПМСД" ВМР', 1]]</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>39089416</t>
+          <t>38822156</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>[["КНП ''Сновський ЦПМСД'' СМР", 14], ['КНП «Ічнянська міська лікарня» Ічнянської міської ради', 2]]</t>
+          <t>[['КНП "Березівський міський ЦПМСД"', 12], ['кнп "Березівський міський ЦПМСД"', 1]]</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>39115875</t>
+          <t>38860558</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>[['ТОВ "КСТ"Фемелі мед клінік"вул. Лізи Чайкіної 69', 6], ['ТОВ "КСТ"Фемелі мед клінік"вул. Лізи Чайкіної 70', 1], ['ТОВ "КСТ"Фемелі мед клінік"вул. Лізи Чайкіної 74', 1]]</t>
+          <t>[["КНП '' Лосинівський ЦПМСД'' ЛСР", 20], ["КНП ''Ніжинський міський ЦПМСД'' НМР", 8], ["КНП ''Ічнянський ЦПМСД'' ІМР", 2]]</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>40081352</t>
+          <t>39042509</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>[['дніпровська КЛ на залізничному транспорті', 11], ['Львівська клінічна лікарня на залізничному транспорті філії "ЦОЗ" АТ "Укрзалізниця"', 10], ['ХАРКІВСЬКА КЛІНІЧНА ЛІКАРНЯ НА ЗАЛІЗНИЧНОМУ ТРАНСПОРТІ №2 ФІЛІЇ "ЦЕНТР ОХОРОНИ ЗДОРОВ\'Я" АКЦІОНЕРНОГО ТОВАРИСТВА "УКРАЇНСЬКА ЗАЛІЗНИЦЯ"', 1]]</t>
+          <t>[['КНП "Андрушівський ЦПМСД"', 8], ['КНП "ЦПМСД" Андрушівська м/р', 8]]</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>40208847</t>
+          <t>39089416</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>[['ЦПМСД Ушомирської ср', 6], ['КНП ЦПМСД Ушомирської с/р', 4]]</t>
+          <t>[["КНП ''Сновський ЦПМСД'' СМР", 14], ['КНП «Ічнянська міська лікарня» Ічнянської міської ради', 2]]</t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>40333372</t>
+          <t>40081352</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>[['КНП"ЦПМСД Чорноострівської селищної ради"', 2], ['КНП ЦПМСД Чорноострівської селищної ради', 1], ['КНП ЦПМСД Чорний Острів', 1], ['КНП ЦПМСД Чорний ОСТРІВ', 1], ['КНП ЦПМСД ЧорнийОстрів', 2], ['КНП ЦПМСД ЧОРНООСТРІВСЬКОЇ селищної ради', 1], ["КНП''ЦПМСД ЧОРНИЙ ОСТРІВ''", 1]]</t>
+          <t>[['дніпровська КЛ на залізничному транспорті', 11], ['Львівська клінічна лікарня на залізничному транспорті філії "ЦОЗ" АТ "Укрзалізниця"', 10], ['ХАРКІВСЬКА КЛІНІЧНА ЛІКАРНЯ НА ЗАЛІЗНИЧНОМУ ТРАНСПОРТІ №2 ФІЛІЇ "ЦЕНТР ОХОРОНИ ЗДОРОВ\'Я" АКЦІОНЕРНОГО ТОВАРИСТВА "УКРАЇНСЬКА ЗАЛІЗНИЦЯ"', 4]]</t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>40382938</t>
+          <t>40208847</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>[["ТОВ''МЦЗР''100 відсотків життя''", 11], ["ТОВ ''Медичиний центр здоров'я та реабілітації '' 100 відсотків життя''", 6]]</t>
+          <t>[['ЦПМСД Ушомирської ср', 8], ['КНП ЦПМСД Ушомирської с/р', 5]]</t>
         </is>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>40407915</t>
+          <t>40333372</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>[['МЕДКОМ', 11], ['МЕДКОМ Березне', 7]]</t>
+          <t>[['КНП"ЦПМСД Чорноострівської селищної ради"', 2], ['КНП ЦПМСД Чорноострівської селищної ради', 1], ['КНП ЦПМСД Чорний Острів', 1], ['КНП ЦПМСД Чорний ОСТРІВ', 1], ['КНП ЦПМСД ЧорнийОстрів', 2], ['КНП ЦПМСД ЧОРНООСТРІВСЬКОЇ селищної ради', 1], ["КНП''ЦПМСД ЧОРНИЙ ОСТРІВ''", 1]]</t>
         </is>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>40595597</t>
+          <t>40382938</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>[['КНП "ЦПМСД Меджибізької СР"', 4], ['КНП " Меджибізької СР"', 1], ['"КНП ЦПМСД Меджибізької СР"', 1]]</t>
+          <t>[["ТОВ''МЦЗР''100 відсотків життя''", 11], ["ТОВ ''Медичиний центр здоров'я та реабілітації '' 100 відсотків життя''", 6]]</t>
         </is>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>40887956</t>
+          <t>40407915</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>[['КП"ХМЦПМСД №2"', 2], ['КП"ХМЦПМСД№2"', 6], ['ХМЦПМСД№2"', 1]]</t>
+          <t>[['МЕДКОМ', 10], ['МЕДКОМ Березне', 7]]</t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>40992563</t>
+          <t>40595597</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>[['КНП"ЦПМСД"Сатанівської селищної ради', 13], ['КНП "ЦПМСД"Сатанівської селищної ради', 1]]</t>
+          <t>[['КНП "ЦПМСД Меджибізької СР"', 4], ['КНП " Меджибізької СР"', 1], ['"КНП ЦПМСД Меджибізької СР"', 1]]</t>
         </is>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>41140764</t>
+          <t>40887956</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>[['ТОВ "Приватна поліклініка ПрофіМед"', 8], ['ПП"Приватна поліклініка "Малятко плюс"', 5]]</t>
+          <t>[['КП"ХМЦПМСД №2"', 2], ['КП"ХМЦПМСД№2"', 8], ['ХМЦПМСД№2"', 1]]</t>
         </is>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>41750747</t>
+          <t>40992563</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>[["КНП '' ЦПМСД Наркевицької СР ''", 3], ['КНП " ЦПМСД Наркевицької СР"', 1], ['КНП "ЦПМСД Наркевицької СР"', 4], ['КНП " ЦПМСД Наркевицької СР "', 1]]</t>
+          <t>[['КНП"ЦПМСД"Сатанівської селищної ради', 13], ['КНП "ЦПМСД"Сатанівської селищної ради', 1]]</t>
         </is>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>41774140</t>
+          <t>41140764</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>[['КП " Медичний лікувально-діагностичний центр " с.Кулевча', 6], ['КП"Медичний лікувально-діагностичний центр" с.Кулевча', 2], ['КП"Медичний лікувально-діагностичний центр"', 1]]</t>
+          <t>[['ТОВ "Приватна поліклініка ПрофіМед"', 8], ['ПП"Приватна поліклініка "Малятко плюс"', 5]]</t>
         </is>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>41877252</t>
+          <t>41750747</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>[['КНП ЦПМСД Полонської міської ради', 10], ['ІКНП ЦПМСД Полонської міської ради', 1]]</t>
+          <t>[["КНП '' ЦПМСД Наркевицької СР ''", 3], ['КНП " ЦПМСД Наркевицької СР"', 1], ['КНП "ЦПМСД Наркевицької СР"', 4], ['КНП " ЦПМСД Наркевицької СР "', 1]]</t>
         </is>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>41940690</t>
+          <t>41774140</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>[['Комунальне некомерційне підприємство "Довбиський селищний Центр первинної медико-санітарної допомоги"Довбиської селищної ради', 9], ['КНП "Довбиський селищний ЦПМСД"Довбиської селищної ради', 1]]</t>
+          <t>[['КП " Медичний лікувально-діагностичний центр " с.Кулевча', 6], ['КП"Медичний лікувально-діагностичний центр" с.Кулевча', 2], ['КП"Медичний лікувально-діагностичний центр"', 1]]</t>
         </is>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>41995294</t>
+          <t>41877252</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>[['КНП "ЦПМСД\' Ямницької сільської ради', 6], ['КНП "ЦПМСД" Ямницької сільської ради', 9]]</t>
+          <t>[['КНП ЦПМСД Полонської міської ради', 10], ['ІКНП ЦПМСД Полонської міської ради', 1]]</t>
         </is>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>42002686</t>
+          <t>41940690</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>[['КНП НМР Центр ПМСД', 10], ['КНП НМР "Центр ПМСД"', 1]]</t>
+          <t>[['Комунальне некомерційне підприємство "Довбиський селищний Центр первинної медико-санітарної допомоги"Довбиської селищної ради', 8], ['КНП "Довбиський селищний ЦПМСД"Довбиської селищної ради', 1]]</t>
         </is>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>42241755</t>
+          <t>41995294</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>[['КНП «ЦПМСД Березанської міської ради»', 8], ['КНП "Березанський РЦ ПМСД"', 15]]</t>
+          <t>[['КНП "ЦПМСД\' Ямницької сільської ради', 6], ['КНП "ЦПМСД" Ямницької сільської ради', 9]]</t>
         </is>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>42273991</t>
+          <t>42002686</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>[['ТОВ " Медикал Сервіс"', 5], ['Медичний центр ТОВ "Медикал-Сервіс"', 8], ['ТОВ "Медикал сервіс\'\'', 12]]</t>
+          <t>[['КНП НМР Центр ПМСД', 9], ['КНП НМР "Центр ПМСД"', 1]]</t>
         </is>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>42277419</t>
+          <t>42241755</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>[['КНП "Шепетівський міський центр ПМСД" Шепетівської ради', 5], ['КНП Шепетівський МЦ ПМСД', 1]]</t>
+          <t>[['КНП «ЦПМСД Березанської міської ради»', 8], ['КНП "Березанський РЦ ПМСД"', 15]]</t>
         </is>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>42500117</t>
+          <t>42273991</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>[['КНП "Центр первинної медико-санітарної допомоги" Южненської міської ради', 5], ['кНП "Центр первинної медико-санітарної допомоги" Южненської міської ради', 1]]</t>
+          <t>[['ТОВ " Медикал Сервіс"', 5], ['Медичний центр ТОВ "Медикал-Сервіс"', 8], ['ТОВ "Медикал сервіс\'\'', 12]]</t>
         </is>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>42579187</t>
+          <t>42277419</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>[['КНП "ЦПМСД" ГУМЕНЕЦЬКОЇ СР', 1], ['КНП "ЦПМСД" Гуменецької СР', 12]]</t>
+          <t>[['КНП "Шепетівський міський центр ПМСД" Шепетівської ради', 6], ['КНП Шепетівський МЦ ПМСД', 1]]</t>
         </is>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>43561851</t>
+          <t>42487175</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>[['ТОВ" Перша приватна поліклініка Миколаїв"', 2], ['ТОВ "Перша приватна полклініка Миколаїва"', 19]]</t>
+          <t>[['КНП" Чоповицький СЦПМСД"Чоповицької селищної ради', 2], ['КНП" ЧоповицькийСЦПМСД"Чоповицької селищної ради', 12]]</t>
         </is>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>43575733</t>
+          <t>42579187</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>[['ТОВ Медична Зірка', 12], ['ТОВ «Медична Зірка»', 9]]</t>
+          <t>[['КНП "ЦПМСД" ГУМЕНЕЦЬКОЇ СР', 1], ['КНП "ЦПМСД" Гуменецької СР', 12]]</t>
         </is>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>43731768</t>
+          <t>42739284</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>[['ТОВ "КСМ"Біхелсі""', 16], ['ТзОВ «КСМ Біхелсі»', 11]]</t>
+          <t>[['КНП "Народицька лікарня" Народицької селищної ради', 2], ['КНП "ЦПМСД" Народицької селищної ради', 2]]</t>
         </is>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>43762272</t>
+          <t>43575733</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>[['ТОВ МЦ Лікарська династія', 13], ['ТОВ "Медичний центр "Лікарська династія"', 10]]</t>
+          <t>[['ТОВ Медична Зірка', 12], ['ТОВ «Медична Зірка»', 9]]</t>
         </is>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>43778764</t>
+          <t>43731768</t>
         </is>
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>[['ТОВ "Медикал плюс"', 4], ['ТзОВ «Медікал плюс»', 5]]</t>
+          <t>[['ТОВ "КСМ"Біхелсі""', 18], ['ТзОВ «КСМ Біхелсі»', 12]]</t>
         </is>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>43858467</t>
+          <t>43762272</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>[['ТОВ "Первинка - 2"', 13], ['ТОВ "МЦ "Первинка-2"', 8]]</t>
+          <t>[['ТОВ МЦ Лікарська династія', 14], ['ТОВ "Медичний центр "Лікарська династія"', 10]]</t>
         </is>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>43871190</t>
+          <t>43778764</t>
         </is>
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>[['ТОВ "Нова Поліклініка Захід"', 12], ['ТОВ «Нова Поліклініка»', 9]]</t>
+          <t>[['ТОВ "Медикал плюс"', 4], ['ТзОВ «Медікал плюс»', 5]]</t>
         </is>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>44040634</t>
+          <t>43858467</t>
         </is>
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>[['КНП «Житомирська багатопрофільна опорна лікарня» Новогуйвинської сел. ради', 2], ['Комунальне некомерційне підприємство "Амбулаторія загальної практики-сімейної медицини" Барашівської сільської ради', 5]]</t>
+          <t>[['ТОВ "Первинка - 2"', 13], ['ТОВ "МЦ "Первинка-2"', 9]]</t>
         </is>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
+          <t>43871190</t>
+        </is>
+      </c>
+      <c r="B91" t="inlineStr">
+        <is>
+          <t>[['ТОВ "Нова Поліклініка Захід"', 12], ['ТОВ «Нова Поліклініка»', 9]]</t>
+        </is>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="inlineStr">
+        <is>
+          <t>44040634</t>
+        </is>
+      </c>
+      <c r="B92" t="inlineStr">
+        <is>
+          <t>[['КНП «Житомирська багатопрофільна опорна лікарня» Новогуйвинської сел. ради', 2], ['Комунальне некомерційне підприємство "Амбулаторія загальної практики-сімейної медицини" Барашівської сільської ради', 8]]</t>
+        </is>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="inlineStr">
+        <is>
           <t>5483121</t>
         </is>
       </c>
-      <c r="B91" t="inlineStr">
+      <c r="B93" t="inlineStr">
         <is>
           <t>[['МДЛ№2', 12], ['MДЛ№2', 1]]</t>
         </is>

</xml_diff>

<commit_message>
2024-04-05 Update. Bug fixes and enhanced data-generating program's verbosity
</commit_message>
<xml_diff>
--- a/Results/Коди ЄДРПОУ з багатьма варіантами назв закладів.xlsx
+++ b/Results/Коди ЄДРПОУ з багатьма варіантами назв закладів.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B93"/>
+  <dimension ref="A1:B95"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -453,7 +453,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>[['КНП"ЖовтоводськаМЛ"', 3], ['КНП"Жовтоводська МЛ"ЖМР', 1]]</t>
+          <t>[['КНП"ЖовтоводськаМЛ"', 4], ['КНП"Жовтоводська МЛ"ЖМР', 2]]</t>
         </is>
       </c>
     </row>
@@ -477,7 +477,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>[['КНП"БЛІЛ КМР"', 5], ['КНП"БЛІЛ КМР', 1]]</t>
+          <t>[['КНП"БЛІЛ КМР"', 4], ['КНП"БЛІЛ КМР', 1]]</t>
         </is>
       </c>
     </row>
@@ -508,1044 +508,1068 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>1998785</t>
+          <t>1998383</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>[['КНП "Кодимська лікарня" Кодимської міської ради Подільського району Одеської області', 2], ['КНП "Кодимська лікарня"\n  Кодимської міської ради\n  Подільського району\n  Одеської області', 2]]</t>
+          <t>[['КНП" МОКЛ"', 1], ['КНК"МОКЛ"', 1]]</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>2004216</t>
+          <t>1998785</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>[['КНП "Городоцька МБЛ" Городоцької міської ради', 1], ['КНП "Городоцька МБЛ"', 2]]</t>
+          <t>[['КНП "Кодимська лікарня" Кодимської міської ради Подільського району Одеської області', 2], ['КНП "Кодимська лікарня"\n  Кодимської міської ради\n  Подільського району\n  Одеської області', 2]]</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>2004350</t>
+          <t>2004216</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>[['КНП"КрасилівськаБЛ"', 1], ['КНП "Красилівська БЛ"', 1], ['КНП"Красилівська БЛ"', 1]]</t>
+          <t>[['КНП "Городоцька МБЛ" Городоцької міської ради', 1], ['КНП "Городоцька МБЛ"', 2]]</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>2004367</t>
+          <t>2004350</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>[['КНА "Летичівська багатопрорфільна лікарня"', 1], ['КРП "Летичівська багатопрофільна лікарня"', 1]]</t>
+          <t>[['КНП"КрасилівськаБЛ"', 1], ['КНП "Красилівська БЛ"', 1], ['КНП"Красилівська БЛ"', 1]]</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>2004404</t>
+          <t>2004367</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>[['КНП "Полонська МЛ ім. Н. С. Говорун"', 2], ['Комунальне некомерційне підприємство Полонської міської ради "Полонська міська багатопрофільна лікарня ім. Наталії Савеліївни Говорун"', 1]]</t>
+          <t>[['КНА "Летичівська багатопрорфільна лікарня"', 1], ['КРП "Летичівська багатопрофільна лікарня"', 1]]</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>2004746</t>
+          <t>2004404</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>[['КП " Хмельницький міський перинатальний центр"', 1], ['КП "Хмельницький міський перинатальний центр"', 2]]</t>
+          <t>[['Комунальне некомерційне підприємство Полонської міської ради "Полонська міська багатопрофільна лікарня ім. Наталії Савеліївни Говорун"', 1], ['КНП "Полонська МЛ ім. Н. С. Говорун"', 1]]</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>2004812</t>
+          <t>2004746</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>[['КНП "Шепетівська багатопрофільна лікарня" Шепетівської міської ради', 2], ['КНП "Шепетівська багатопофільна лікарня" Шепетівської міської ради', 1], ['КНП"Шепетівська багатопрофільна лікарня" Шепетівської міської ради', 1]]</t>
+          <t>[['КП " Хмельницький міський перинатальний центр"', 1], ['КП "Хмельницький міський перинатальний центр"', 2]]</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>2006194</t>
+          <t>2004812</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>[["КНП ''Коропська ЦЛ'' КСР", 1], ['КНП «Варвинська лікарня» Варвинської селищної ради Прилуцького району Чернігівської області', 1]]</t>
+          <t>[['КНП "Шепетівська багатопрофільна лікарня" Шепетівської міської ради', 2], ['КНП "Шепетівська багатопофільна лікарня" Шепетівської міської ради', 1], ['КНП"Шепетівська багатопрофільна лікарня" Шепетівської міської ради', 1]]</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>2006225</t>
+          <t>2006194</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>[["КНП ''Городнянська МЛ'' ГМР", 12], ["КНП ''Корюківська ЦРЛ'' КМР", 4]]</t>
+          <t>[["КНП ''Коропська ЦЛ'' КСР", 1], ['КНП «Варвинська лікарня» Варвинської селищної ради Прилуцького району Чернігівської області', 1]]</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>2006604</t>
+          <t>2006225</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>[["КНП ''Сновська ЦРЛ'' СМР", 1], ["КНП ''Прилуцька міська дитяча лікарня'' ПМР", 5]]</t>
+          <t>[["КНП ''Городнянська МЛ'' ГМР", 12], ["КНП ''Корюківська ЦРЛ'' КМР", 4]]</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>2006610</t>
+          <t>2006604</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>[["КНП ''Чернігівська МЛ №4'' ЧМР", 5], ['КНП «Пологовий будинок» Чернігівської міської ради', 2]]</t>
+          <t>[["КНП ''Сновська ЦРЛ'' СМР", 1], ["КНП ''Прилуцька міська дитяча лікарня'' ПМР", 5]]</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>2148517983</t>
+          <t>2006610</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>[['ФОП Олійник Д.Д.', 8], ['ФОП ОЛійник Д.Д.', 1], ['ФОП олійник Д.Д.', 1]]</t>
+          <t>[["КНП ''Чернігівська МЛ №4'' ЧМР", 5], ['КНП «Пологовий будинок» Чернігівської міської ради', 2]]</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>22348948</t>
+          <t>2148517983</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>[['БФ ім. Митрополита А. Шептицького', 6], ['Благодійний Фонд "Шпиталь імені Митрополита Андрея Шептицького Курії Львівської Архиєпархії Української Греко-Католицької Церкви"', 12]]</t>
+          <t>[['ФОП Олійник Д.Д.', 9], ['ФОП ОЛійник Д.Д.', 1], ['ФОП олійник Д.Д.', 1]]</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>2314026147</t>
+          <t>22348948</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>[['ФОП Селезньова С. Л', 3], ['ФОП Селезньова С.Л', 3]]</t>
+          <t>[['БФ ім. Митрополита А. Шептицького', 5], ['Благодійний Фонд "Шпиталь імені Митрополита Андрея Шептицького Курії Львівської Архиєпархії Української Греко-Католицької Церкви"', 12]]</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>2339913111</t>
+          <t>2314026147</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>[['ФОП "Сем\'янчук В.Б."', 9], ['ФОП Білик Роман Павлович', 10]]</t>
+          <t>[['ФОП Селезньова С. Л', 4], ['ФОП Селезньова С.Л', 3]]</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>26381838</t>
+          <t>2339913111</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>[['КНП " Дитячий МЦ" КПМР', 10], ['КНП " Дитячий МЦ " КПМР', 2]]</t>
+          <t>[['ФОП "Сем\'янчук В.Б."', 9], ['ФОП Білик Роман Павлович', 10]]</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>2727016128</t>
+          <t>26381838</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>[['ФОП Ковенько Т.', 8], ['ФОП КовенькоТ.', 3]]</t>
+          <t>[['КНП " Дитячий МЦ" КПМР', 10], ['КНП " Дитячий МЦ " КПМР', 2]]</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>2774384</t>
+          <t>2727016128</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>[['КП " Хмельницька міська лікарня"', 1], ['КП "Хмльницька міська лікарня"', 1], ['комунальне підприємство "Хмельницька міська лікарня " Хмельницької міської ради', 1], ['комунальне підприємство  " Хмельницька міська лікарня" Хмельницької міської ради', 1]]</t>
+          <t>[['ФОП Ковенько Т.', 6], ['ФОП КовенькоТ.', 3]]</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>2798817680</t>
+          <t>2774384</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>[['ФОП Слободянюк Л.А.', 43], ['фОП Слободянюк Л.А.', 1], ['ФОП Слободянюк Л.А. педіатр', 110]]</t>
+          <t>[['КП " Хмельницька міська лікарня"', 1], ['КП "Хмльницька міська лікарня"', 1], ['комунальне підприємство "Хмельницька міська лікарня " Хмельницької міської ради', 1], ['комунальне підприємство  " Хмельницька міська лікарня" Хмельницької міської ради', 1]]</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>2939705320</t>
+          <t>2798817680</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>[['ПП "Віва Клінік"', 5], ['ПП "Віва Клінік" м.Славута', 2], ['ПП " Віва Клінік"', 5]]</t>
+          <t>[['ФОП Слободянюк Л.А.', 43], ['фОП Слободянюк Л.А.', 1], ['ФОП Слободянюк Л.А. педіатр', 117]]</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>2975100945</t>
+          <t>2939705320</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>[['ФОП Ковтун Людмила Володимирівна', 11], ['фОП Ковтун Людмила Володимирівна', 1]]</t>
+          <t>[['ПП "Віва Клінік"', 5], ['ПП "Віва Клінік" м.Славута', 2], ['ПП " Віва Клінік"', 5]]</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>3146414401</t>
+          <t>2975100945</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>[['ФОП Робейко Фаїна Олександрівна', 7], ['ФОП Робейко Фауна Олександрівна', 1]]</t>
+          <t>[['ФОП Ковтун Людмила Володимирівна', 11], ['фОП Ковтун Людмила Володимирівна', 1]]</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>3153200965</t>
+          <t>3146414401</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>[['ФОП ГУЗАК ОІ', 6], ['ФОп ГУЗАК ОІ', 1]]</t>
+          <t>[['ФОП Робейко Фаїна Олександрівна', 7], ['ФОП Робейко Фауна Олександрівна', 1]]</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>3210314064</t>
+          <t>3198123020</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>[['Фоп Осипенко К.В', 3], ['ФОП  Осипенко К.В', 1]]</t>
+          <t>[['ФОП Лавренчук Ірина Олегівна', 11], ['Обухівський район ФОП Лавренчук Ірина Олегівна', 11]]</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>3259514282</t>
+          <t>3210314064</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>[['ФОП Віннічук Юлія Валеріївна', 3], ['ФОП Віннічук Ю.В.', 20], ['ФОП ВІннічук Ю.В.', 3], ['ФОП ВІНнічук Ю.В.', 1]]</t>
+          <t>[['Фоп Осипенко К.В', 3], ['ФОП  Осипенко К.В', 1]]</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>3280718060</t>
+          <t>3259514282</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>[['ФОП Гончар Інна Михайлівна', 6], ['Фоп ГоНЧАР ІМ', 1], ['Фоп ГОНЧАР ІМ', 1], ['ФОП ГОНЧАР ІМ', 4]]</t>
+          <t>[['ФОП Віннічук Юлія Валеріївна', 3], ['ФОП Віннічук Ю.В.', 20], ['ФОП ВІннічук Ю.В.', 7], ['ФОП ВІНнічук Ю.В.', 1]]</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>35479197</t>
+          <t>3280718060</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>[['ТОВ Клініка Свій лікар м.Дунаївці', 1], ['ТОВ"КЛІНІКА СВІЙ ЛІКАР"м.Дунаївці', 6], ['ПП"Сіліцея"', 7]]</t>
+          <t>[['ФОП Гончар Інна Михайлівна', 6], ['Фоп ГоНЧАР ІМ', 1], ['Фоп ГОНЧАР ІМ', 1], ['ФОП ГОНЧАР ІМ', 4]]</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>37263866</t>
+          <t>3284623415</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>[['ПП"Приватна поліклініка "Малятко плюс"', 45], ['ПП "Малятко плюс"', 25], ['ПП"Малятко плюс"', 20]]</t>
+          <t>[['Білоцерківський район ФОП Ленчук Андрій Станіславович', 8], ['Білоцерківський район ФОП Піщана Надія Юріївна', 3]]</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>37329345</t>
+          <t>3320813521</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>[['КНП"СТАРОСИНЯВСЬКИЙ ЦПМСД"', 3], ['КНП СТАРОСИНЯВСЬКИЙ ЦПМСД', 7], ['КНП "СТАРОСИНЯВСЬКИЙ ЦПМСД"', 1]]</t>
+          <t>[['Білоцерківський район ФОП Гальчинський Олександр Олегович', 1], ['Білоцерківський район ФОП Піщана Надія Юріївна', 6]]</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>37803420</t>
+          <t>33761466</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>[['КНП "Мирноградський центр первинної медико-санітарної допомоги"', 1], ['КНП "Мирноградський центр первинної медико-санітарної допомоги "', 10], ['КНП " Мирноградський центр первинної медико-санітарної допомоги"', 1]]</t>
+          <t>[['Приватне підприємство "МІЛАМЕД"', 5], ['Приватне підприємство " МІЛАМЕД"', 2]]</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>38073028</t>
+          <t>35479197</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>[["КНП ''Городнянський ЦПМСД'' ГМР", 13], ["КНП '' Семенівський ЦПМСД'' СМР", 3]]</t>
+          <t>[['ТОВ Клініка Свій лікар м.Дунаївці', 1], ['ТОВ"КЛІНІКА СВІЙ ЛІКАР"м.Дунаївці', 6], ['ПП"Сіліцея"', 7]]</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>38195242</t>
+          <t>37263866</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>[['КНП «Деражнянський ЦПМСД» ДМР ХО', 9], ['КПН "Деражнянський ЦПМСД"ДМР ХО', 1]]</t>
+          <t>[['ПП"Приватна поліклініка "Малятко плюс"', 45], ['ПП "Малятко плюс"', 25], ['ПП"Малятко плюс"', 26]]</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>38195551</t>
+          <t>37329345</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>[['КНП "КНП Чемеровецький центр ПМСД"', 1], ['КНП "Чемеровецький центр ПМСД"', 6], ['ТОВ "АЛМ-Поділля"', 3], ['КНП Чемеровецький центр ПМСД', 4]]</t>
+          <t>[['КНП"СТАРОСИНЯВСЬКИЙ ЦПМСД"', 3], ['КНП СТАРОСИНЯВСЬКИЙ ЦПМСД', 7], ['КНП "СТАРОСИНЯВСЬКИЙ ЦПМСД"', 1]]</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>38270455</t>
+          <t>37803420</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>[['КНП "Летичівський ЦПМСД"', 8], ['КНП"Летичівський ЦПМСД" Летичівської селищної ради', 2]]</t>
+          <t>[['КНП "Мирноградський центр первинної медико-санітарної допомоги"', 1], ['КНП "Мирноградський центр первинної медико-санітарної допомоги "', 10], ['КНП " Мирноградський центр первинної медико-санітарної допомоги"', 1]]</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>38281797</t>
+          <t>38073028</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>[['КНП"Новоронцовський районний ЦПМСД"', 10], ['КНП"Новоронцовський районний ЦПМСД"(СКЛАД)', 1]]</t>
+          <t>[["КНП ''Городнянський ЦПМСД'' ГМР", 13], ["КНП '' Семенівський ЦПМСД'' СМР", 3]]</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>38283239</t>
+          <t>38195242</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>[['КНП "Ярмолинецький центр ПМСД"', 6], ['КНП "Ярмолинецький центр ПМСД" ЯСР ХО', 1]]</t>
+          <t>[['КНП «Деражнянський ЦПМСД» ДМР ХО', 9], ['КПН "Деражнянський ЦПМСД"ДМР ХО', 1]]</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>38297440</t>
+          <t>38195551</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>[['КНП "Білогірський ЦПМСД"', 6], ['КНП "БІЛОГІРСЬКИЙ ЦПМСД"', 4]]</t>
+          <t>[['КНП "КНП Чемеровецький центр ПМСД"', 1], ['КНП "Чемеровецький центр ПМСД"', 6], ['ТОВ "АЛМ-Поділля"', 3], ['КНП Чемеровецький центр ПМСД', 4]]</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>38313933</t>
+          <t>38270455</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>[['КП"Первомайський РЦПМСД', 10], ['КОМУНАЛЬНЕ ПІДПРИЄМСТВО «КАМ’ЯНОПО\xadТОКІВСЬКИЙ ЦЕНТР ПЕРВИННОЇ МЕДИКО-САНІТАРНОЇ ДОПОМОГИ»', 9]]</t>
+          <t>[['КНП "Летичівський ЦПМСД"', 7], ['КНП"Летичівський ЦПМСД" Летичівської селищної ради', 2]]</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>38331800</t>
+          <t>38281797</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>[['ДУ Івано-Франківський ОЦКПХ', 11], ['Снятинський відділ', 8]]</t>
+          <t>[['КНП"Новоронцовський районний ЦПМСД"', 9], ['КНП"Новоронцовський районний ЦПМСД"(СКЛАД)', 1]]</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>38341981</t>
+          <t>38283239</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>[['КНП "Бузький РЦ ПСМД"', 8], ['КНП "Бузький РЦ ПМСД"', 1], ['КНП " Бузький ПМСД"', 6]]</t>
+          <t>[['КНП "Ярмолинецький центр ПМСД"', 6], ['КНП "Ярмолинецький центр ПМСД" ЯСР ХО', 1]]</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>38363607</t>
+          <t>38297440</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>[['КНП"Братський ЦПМСД"', 10], ['кнп "Братський ЦПМСД"', 1]]</t>
+          <t>[['КНП "Білогірський ЦПМСД"', 6], ['КНП "БІЛОГІРСЬКИЙ ЦПМСД"', 4]]</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>38402043</t>
+          <t>38313933</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>[['КП КНП Шепетівський Центр ПМСД', 1], ['КП "КПН Шепетівський Центр ПМСД"', 3], ['КП"КНП Шепетівський ЦентрПМСД', 2], ['КП"КНП Шепетівський Центр ПМСД"', 6], ['КП "КНП Шепетівський Центр ПМСД"', 7], ['КП "КНП Шепетівський Центр ПМСД', 4]]</t>
+          <t>[['КП"Первомайський РЦПМСД', 11], ['КОМУНАЛЬНЕ ПІДПРИЄМСТВО «КАМ’ЯНОПО\xadТОКІВСЬКИЙ ЦЕНТР ПЕРВИННОЇ МЕДИКО-САНІТАРНОЇ ДОПОМОГИ»', 11]]</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>38453281</t>
+          <t>38341981</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>[["КНП ''Борзнянський ЦПМСД'' БМР", 5], ["КНП ''Прилуцький міський ЦПМСД''", 2]]</t>
+          <t>[['КНП "Бузький РЦ ПМСД"', 2], ['КНП "Бузький РЦ ПСМД"', 7], ['КНП " Бузький ПМСД"', 6]]</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>38458316</t>
+          <t>38363607</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>[['ДУ "Миколаївський ОЦКПХ"', 4], ['ДУ"Миколаївський ОЦКПХ', 6]]</t>
+          <t>[['КНП"Братський ЦПМСД"', 12], ['кнп "Братський ЦПМСД"', 1]]</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>38469307</t>
+          <t>38402043</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>[['КНП "Центр ПМД Хмельницького району"', 12], ['КНП "ЦПМД Хмельницького району"', 1]]</t>
+          <t>[['КП КНП Шепетівський Центр ПМСД', 1], ['КП "КПН Шепетівський Центр ПМСД"', 3], ['КП"КНП Шепетівський ЦентрПМСД', 2], ['КП"КНП Шепетівський Центр ПМСД"', 5], ['КП "КНП Шепетівський Центр ПМСД"', 7], ['КП "КНП Шепетівський Центр ПМСД', 3]]</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>38474592</t>
+          <t>38453281</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>[['ПП МЕДТОРГ -ЕКСПРЕС', 10], ['ДУ "Волинський обласний центр контролю та профілактики хвороб Міністерства охорони здоров\'я України" (обласний склад)', 6]]</t>
+          <t>[["КНП ''Борзнянський ЦПМСД'' БМР", 5], ["КНП ''Прилуцький міський ЦПМСД''", 2]]</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>38487677</t>
+          <t>38458316</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>[['КНП"Старокостянтинівський ЦПМСД"', 6], ['КНП "Старокостянтинівський ЦПМСД"', 3]]</t>
+          <t>[['ДУ "Миколаївський ОЦКПХ"', 3], ['ДУ"Миколаївський ОЦКПХ', 6]]</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>38500472</t>
+          <t>38469307</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>[['КНП "ЦПМСД" Черняхівської селищної ради', 4], ['КНП "ЦПМСД"Черняхівської селищної ради', 7]]</t>
+          <t>[['КНП "Центр ПМД Хмельницького району"', 12], ['КНП "ЦПМД Хмельницького району"', 1]]</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>38566219</t>
+          <t>38474592</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>[['КНП "Центр ПМСД" КПМР', 10], ['КНП"Центр ПМСД" КПМР', 1]]</t>
+          <t>[['ПП МЕДТОРГ -ЕКСПРЕС', 9], ['ДУ "Волинський обласний центр контролю та профілактики хвороб Міністерства охорони здоров\'я України" (обласний склад)', 6]]</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>38584683</t>
+          <t>38487677</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>[["КНП '' Козелецький ЦПМСД'' КРР", 10], ["КНП ''Сосницький ЦПМСД'' ССР", 1]]</t>
+          <t>[['КНП"Старокостянтинівський ЦПМСД"', 6], ['КНП "Старокостянтинівський ЦПМСД"', 3]]</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>38584715</t>
+          <t>38500472</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>[["КНП ''Новгород-Сіверський міський ЦПМСД'' Н.-Сіверської МР", 7], ["КНП ''Коропський ЦПМСД'' КСР", 1]]</t>
+          <t>[['КНП "ЦПМСД" Черняхівської селищної ради', 3], ['КНП "ЦПМСД"Черняхівської селищної ради', 6]]</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>38611140</t>
+          <t>38566219</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>[['КНП Теофіпольський ЦПСМД', 4], ['КНП "ТЕОФІПОЛЬСЬКИЙ ЦПМСД"', 1], ['Теофіпольський ЦПСМД', 1], ['КНП Теофіпольський ЦПМСД', 4], ['КПН Теофіпольський ЦПМСД', 1]]</t>
+          <t>[['КНП "Центр ПМСД" КПМР', 10], ['КНП"Центр ПМСД" КПМР', 1]]</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>38731750</t>
+          <t>38584683</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>[['КНП "ЦПМСД" Радомишльської міської ради', 10], ['КНП "АЗПСМ"Курненської сільської ради', 2], ['Комунальне некомерційне підприємство "Центр первинної медико-санітарної допомоги" Радомишльської міської ради', 2]]</t>
+          <t>[["КНП '' Козелецький ЦПМСД'' КРР", 10], ["КНП ''Сосницький ЦПМСД'' ССР", 1]]</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>38809093</t>
+          <t>38584715</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>[['КНП "Вільнянський ЦПМСД"ВМР', 18], ['КНП "Вільнянський ЦПМСД" ВМР', 1]]</t>
+          <t>[["КНП ''Новгород-Сіверський міський ЦПМСД'' Н.-Сіверської МР", 6], ["КНП ''Коропський ЦПМСД'' КСР", 1]]</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>38822156</t>
+          <t>38611140</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>[['КНП "Березівський міський ЦПМСД"', 12], ['кнп "Березівський міський ЦПМСД"', 1]]</t>
+          <t>[['КНП Теофіпольський ЦПСМД', 4], ['КНП "ТЕОФІПОЛЬСЬКИЙ ЦПМСД"', 1], ['Теофіпольський ЦПСМД', 1], ['КНП Теофіпольський ЦПМСД', 4], ['КПН Теофіпольський ЦПМСД', 1]]</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>38860558</t>
+          <t>38731750</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>[["КНП '' Лосинівський ЦПМСД'' ЛСР", 20], ["КНП ''Ніжинський міський ЦПМСД'' НМР", 8], ["КНП ''Ічнянський ЦПМСД'' ІМР", 2]]</t>
+          <t>[['КНП "АЗПСМ"Курненської сільської ради', 2], ['КНП "ЦПМСД" Радомишльської міської ради', 10], ['Комунальне некомерційне підприємство "Центр первинної медико-санітарної допомоги" Радомишльської міської ради', 2]]</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>39042509</t>
+          <t>38809093</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>[['КНП "Андрушівський ЦПМСД"', 8], ['КНП "ЦПМСД" Андрушівська м/р', 8]]</t>
+          <t>[['КНП "Вільнянський ЦПМСД"ВМР', 18], ['КНП "Вільнянський ЦПМСД" ВМР', 1]]</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>39089416</t>
+          <t>38822156</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>[["КНП ''Сновський ЦПМСД'' СМР", 14], ['КНП «Ічнянська міська лікарня» Ічнянської міської ради', 2]]</t>
+          <t>[['КНП "Березівський міський ЦПМСД"', 13], ['кнп "Березівський міський ЦПМСД"', 1]]</t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>40081352</t>
+          <t>38860558</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>[['дніпровська КЛ на залізничному транспорті', 11], ['Львівська клінічна лікарня на залізничному транспорті філії "ЦОЗ" АТ "Укрзалізниця"', 10], ['ХАРКІВСЬКА КЛІНІЧНА ЛІКАРНЯ НА ЗАЛІЗНИЧНОМУ ТРАНСПОРТІ №2 ФІЛІЇ "ЦЕНТР ОХОРОНИ ЗДОРОВ\'Я" АКЦІОНЕРНОГО ТОВАРИСТВА "УКРАЇНСЬКА ЗАЛІЗНИЦЯ"', 4]]</t>
+          <t>[["КНП '' Лосинівський ЦПМСД'' ЛСР", 19], ["КНП ''Ніжинський міський ЦПМСД'' НМР", 9], ["КНП ''Ічнянський ЦПМСД'' ІМР", 2]]</t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>40208847</t>
+          <t>39042509</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>[['ЦПМСД Ушомирської ср', 8], ['КНП ЦПМСД Ушомирської с/р', 5]]</t>
+          <t>[['КНП "Андрушівський ЦПМСД"', 7], ['КНП "ЦПМСД" Андрушівська м/р', 8]]</t>
         </is>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>40333372</t>
+          <t>39089416</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>[['КНП"ЦПМСД Чорноострівської селищної ради"', 2], ['КНП ЦПМСД Чорноострівської селищної ради', 1], ['КНП ЦПМСД Чорний Острів', 1], ['КНП ЦПМСД Чорний ОСТРІВ', 1], ['КНП ЦПМСД ЧорнийОстрів', 2], ['КНП ЦПМСД ЧОРНООСТРІВСЬКОЇ селищної ради', 1], ["КНП''ЦПМСД ЧОРНИЙ ОСТРІВ''", 1]]</t>
+          <t>[["КНП ''Сновський ЦПМСД'' СМР", 14], ['КНП «Ічнянська міська лікарня» Ічнянської міської ради', 3]]</t>
         </is>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>40382938</t>
+          <t>40081352</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>[["ТОВ''МЦЗР''100 відсотків життя''", 11], ["ТОВ ''Медичиний центр здоров'я та реабілітації '' 100 відсотків життя''", 6]]</t>
+          <t>[['дніпровська КЛ на залізничному транспорті', 11], ['Львівська клінічна лікарня на залізничному транспорті філії "ЦОЗ" АТ "Укрзалізниця"', 10], ['ХАРКІВСЬКА КЛІНІЧНА ЛІКАРНЯ НА ЗАЛІЗНИЧНОМУ ТРАНСПОРТІ №2 ФІЛІЇ "ЦЕНТР ОХОРОНИ ЗДОРОВ\'Я" АКЦІОНЕРНОГО ТОВАРИСТВА "УКРАЇНСЬКА ЗАЛІЗНИЦЯ"', 4]]</t>
         </is>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>40407915</t>
+          <t>40333372</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>[['МЕДКОМ', 10], ['МЕДКОМ Березне', 7]]</t>
+          <t>[['КНП"ЦПМСД Чорноострівської селищної ради"', 2], ['КНП ЦПМСД Чорноострівської селищної ради', 1], ['КНП ЦПМСД Чорний Острів', 1], ['КНП ЦПМСД Чорний ОСТРІВ', 1], ['КНП ЦПМСД ЧорнийОстрів', 2], ['КНП ЦПМСД ЧОРНООСТРІВСЬКОЇ селищної ради', 1], ["КНП''ЦПМСД ЧОРНИЙ ОСТРІВ''", 1]]</t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>40595597</t>
+          <t>40382938</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>[['КНП "ЦПМСД Меджибізької СР"', 4], ['КНП " Меджибізької СР"', 1], ['"КНП ЦПМСД Меджибізької СР"', 1]]</t>
+          <t>[["ТОВ''МЦЗР''100 відсотків життя''", 11], ["ТОВ ''Медичиний центр здоров'я та реабілітації '' 100 відсотків життя''", 6]]</t>
         </is>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>40887956</t>
+          <t>40407915</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>[['КП"ХМЦПМСД №2"', 2], ['КП"ХМЦПМСД№2"', 8], ['ХМЦПМСД№2"', 1]]</t>
+          <t>[['МЕДКОМ', 10], ['МЕДКОМ Березне', 7]]</t>
         </is>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>40992563</t>
+          <t>40595597</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>[['КНП"ЦПМСД"Сатанівської селищної ради', 13], ['КНП "ЦПМСД"Сатанівської селищної ради', 1]]</t>
+          <t>[['КНП "ЦПМСД Меджибізької СР"', 4], ['КНП " Меджибізької СР"', 1], ['"КНП ЦПМСД Меджибізької СР"', 1]]</t>
         </is>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>41140764</t>
+          <t>40887956</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>[['ТОВ "Приватна поліклініка ПрофіМед"', 8], ['ПП"Приватна поліклініка "Малятко плюс"', 5]]</t>
+          <t>[['КП"ХМЦПМСД №2"', 1], ['КП"ХМЦПМСД№2"', 7], ['ХМЦПМСД№2"', 1]]</t>
         </is>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>41750747</t>
+          <t>40992563</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>[["КНП '' ЦПМСД Наркевицької СР ''", 3], ['КНП " ЦПМСД Наркевицької СР"', 1], ['КНП "ЦПМСД Наркевицької СР"', 4], ['КНП " ЦПМСД Наркевицької СР "', 1]]</t>
+          <t>[['КНП"ЦПМСД"Сатанівської селищної ради', 13], ['КНП "ЦПМСД"Сатанівської селищної ради', 1]]</t>
         </is>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>41774140</t>
+          <t>41140764</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>[['КП " Медичний лікувально-діагностичний центр " с.Кулевча', 6], ['КП"Медичний лікувально-діагностичний центр" с.Кулевча', 2], ['КП"Медичний лікувально-діагностичний центр"', 1]]</t>
+          <t>[['ТОВ "Приватна поліклініка ПрофіМед"', 8], ['ПП"Приватна поліклініка "Малятко плюс"', 5]]</t>
         </is>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>41877252</t>
+          <t>41750747</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>[['КНП ЦПМСД Полонської міської ради', 10], ['ІКНП ЦПМСД Полонської міської ради', 1]]</t>
+          <t>[["КНП '' ЦПМСД Наркевицької СР ''", 3], ['КНП " ЦПМСД Наркевицької СР"', 1], ['КНП "ЦПМСД Наркевицької СР"', 4], ['КНП " ЦПМСД Наркевицької СР "', 1]]</t>
         </is>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>41940690</t>
+          <t>41774140</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>[['Комунальне некомерційне підприємство "Довбиський селищний Центр первинної медико-санітарної допомоги"Довбиської селищної ради', 8], ['КНП "Довбиський селищний ЦПМСД"Довбиської селищної ради', 1]]</t>
+          <t>[['КП " Медичний лікувально-діагностичний центр " с.Кулевча', 6], ['КП"Медичний лікувально-діагностичний центр" с.Кулевча', 4]]</t>
         </is>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>41995294</t>
+          <t>41877252</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>[['КНП "ЦПМСД\' Ямницької сільської ради', 6], ['КНП "ЦПМСД" Ямницької сільської ради', 9]]</t>
+          <t>[['КНП ЦПМСД Полонської міської ради', 10], ['ІКНП ЦПМСД Полонської міської ради', 1]]</t>
         </is>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>42002686</t>
+          <t>41995294</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>[['КНП НМР Центр ПМСД', 9], ['КНП НМР "Центр ПМСД"', 1]]</t>
+          <t>[['КНП "ЦПМСД\' Ямницької сільської ради', 5], ['КНП "ЦПМСД" Ямницької сільської ради', 11]]</t>
         </is>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>42241755</t>
+          <t>42002686</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>[['КНП «ЦПМСД Березанської міської ради»', 8], ['КНП "Березанський РЦ ПМСД"', 15]]</t>
+          <t>[['КНП НМР Центр ПМСД', 9], ['КНП НМР "Центр ПМСД"', 1]]</t>
         </is>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>42273991</t>
+          <t>42241755</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>[['ТОВ " Медикал Сервіс"', 5], ['Медичний центр ТОВ "Медикал-Сервіс"', 8], ['ТОВ "Медикал сервіс\'\'', 12]]</t>
+          <t>[['Броварський район КНП «ЦПМСД Березанської міської ради»', 8], ['КНП "Березанський РЦ ПМСД"', 15]]</t>
         </is>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>42277419</t>
+          <t>42273991</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>[['КНП "Шепетівський міський центр ПМСД" Шепетівської ради', 6], ['КНП Шепетівський МЦ ПМСД', 1]]</t>
+          <t>[['Білоцерківський район ТОВ "Медикал Сервіс"', 7], ['Медичний центр ТОВ "Медикал-Сервіс"', 8], ['ТОВ "Медикал сервіс\'\'', 13]]</t>
         </is>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>42487175</t>
+          <t>42277419</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>[['КНП" Чоповицький СЦПМСД"Чоповицької селищної ради', 2], ['КНП" ЧоповицькийСЦПМСД"Чоповицької селищної ради', 12]]</t>
+          <t>[['КНП "Шепетівський міський центр ПМСД" Шепетівської ради', 6], ['КНП Шепетівський МЦ ПМСД', 1]]</t>
         </is>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>42579187</t>
+          <t>42487175</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>[['КНП "ЦПМСД" ГУМЕНЕЦЬКОЇ СР', 1], ['КНП "ЦПМСД" Гуменецької СР', 12]]</t>
+          <t>[['КНП" ЧоповицькийСЦПМСД"Чоповицької селищної ради', 12], ['КНП" Чоповицький СЦПМСД"Чоповицької селищної ради', 1]]</t>
         </is>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>42739284</t>
+          <t>42579187</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>[['КНП "Народицька лікарня" Народицької селищної ради', 2], ['КНП "ЦПМСД" Народицької селищної ради', 2]]</t>
+          <t>[['КНП "ЦПМСД" ГУМЕНЕЦЬКОЇ СР', 1], ['КНП "ЦПМСД" Гуменецької СР', 12]]</t>
         </is>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>43575733</t>
+          <t>42739284</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>[['ТОВ Медична Зірка', 12], ['ТОВ «Медична Зірка»', 9]]</t>
+          <t>[['КНП "Народицька лікарня" Народицької селищної ради', 2], ['КНП "ЦПМСД" Народицької селищної ради', 2]]</t>
         </is>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>43731768</t>
+          <t>42828300</t>
         </is>
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>[['ТОВ "КСМ"Біхелсі""', 18], ['ТзОВ «КСМ Біхелсі»', 12]]</t>
+          <t>[['КНП"Смотрицький центр ПМСД"ССР', 11], ['КНП"Смортицький центр ПМСД"сср', 1]]</t>
         </is>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>43762272</t>
+          <t>43575733</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>[['ТОВ МЦ Лікарська династія', 14], ['ТОВ "Медичний центр "Лікарська династія"', 10]]</t>
+          <t>[['ТОВ Медична Зірка', 12], ['ТОВ «Медична Зірка»', 9]]</t>
         </is>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>43778764</t>
+          <t>43731768</t>
         </is>
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>[['ТОВ "Медикал плюс"', 4], ['ТзОВ «Медікал плюс»', 5]]</t>
+          <t>[['ТОВ "КСМ"Біхелсі""', 17], ['ТзОВ «КСМ Біхелсі»', 12]]</t>
         </is>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>43858467</t>
+          <t>43762272</t>
         </is>
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>[['ТОВ "Первинка - 2"', 13], ['ТОВ "МЦ "Первинка-2"', 9]]</t>
+          <t>[['Обухівський район ТОВ МЦ Лікарська династія', 13], ['ТОВ "Медичний центр "Лікарська династія"', 10]]</t>
         </is>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>43871190</t>
+          <t>43778764</t>
         </is>
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>[['ТОВ "Нова Поліклініка Захід"', 12], ['ТОВ «Нова Поліклініка»', 9]]</t>
+          <t>[['ТОВ "Медикал плюс"', 5], ['ТзОВ «Медікал плюс»', 5]]</t>
         </is>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>44040634</t>
+          <t>43858467</t>
         </is>
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>[['КНП «Житомирська багатопрофільна опорна лікарня» Новогуйвинської сел. ради', 2], ['Комунальне некомерційне підприємство "Амбулаторія загальної практики-сімейної медицини" Барашівської сільської ради', 8]]</t>
+          <t>[['ТОВ "Первинка - 2"', 12], ['ТОВ "МЦ "Первинка-2"', 9]]</t>
         </is>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
+          <t>43871190</t>
+        </is>
+      </c>
+      <c r="B93" t="inlineStr">
+        <is>
+          <t>[['ТОВ "Нова Поліклініка Захід"', 12], ['ТОВ «Нова Поліклініка»', 8]]</t>
+        </is>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="inlineStr">
+        <is>
+          <t>44040634</t>
+        </is>
+      </c>
+      <c r="B94" t="inlineStr">
+        <is>
+          <t>[['КНП «Житомирська багатопрофільна опорна лікарня» Новогуйвинської сел. ради', 2], ['Комунальне некомерційне підприємство "Амбулаторія загальної практики-сімейної медицини" Барашівської сільської ради', 8]]</t>
+        </is>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="inlineStr">
+        <is>
           <t>5483121</t>
         </is>
       </c>
-      <c r="B93" t="inlineStr">
-        <is>
-          <t>[['МДЛ№2', 12], ['MДЛ№2', 1]]</t>
+      <c r="B95" t="inlineStr">
+        <is>
+          <t>[['МДЛ№2', 13], ['MДЛ№2', 1]]</t>
         </is>
       </c>
     </row>

</xml_diff>